<commit_message>
自动更新数据 - 2025-04-28 16:39:59
</commit_message>
<xml_diff>
--- a/data/raw/水晶.xlsx
+++ b/data/raw/水晶.xlsx
@@ -39,6 +39,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ 明朝"/>
+        <charset val="134"/>
+      </rPr>
       <t>翡翠</t>
     </r>
     <r>
@@ -1493,6 +1499,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ 明朝"/>
+        <charset val="134"/>
+      </rPr>
       <t>黄金</t>
     </r>
     <r>
@@ -3064,116 +3076,7 @@
     <t>长石</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>蓝月光</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>，</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>灰月光</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>，</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>橙月光</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>，</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>金太阳</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>，</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>阿鲁沙</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>，</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>星辉骨干</t>
-    </r>
+    <t>蓝月光，灰月光，橙月光，金太阳，阿鲁沙，星辉骨干</t>
   </si>
   <si>
     <t>天河石</t>
@@ -5152,10 +5055,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C156"/>
+  <dimension ref="A1:C157"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" workbookViewId="0">
-      <selection activeCell="A1" sqref="A$1:A$1048576"/>
+    <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="119" topLeftCell="A149" workbookViewId="0">
+      <selection activeCell="B160" sqref="B160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelCol="2"/>
@@ -5176,7 +5079,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" ht="51.75" spans="1:3">
+    <row r="2" ht="17.75" spans="1:3">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -5194,7 +5097,7 @@
       </c>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" ht="51.75" spans="1:3">
+    <row r="4" ht="17.75" spans="1:3">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -5203,7 +5106,7 @@
       </c>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" ht="51.75" spans="1:3">
+    <row r="5" ht="17.75" spans="1:3">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -5212,7 +5115,7 @@
       </c>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" ht="51.75" spans="1:3">
+    <row r="6" ht="17.75" spans="1:3">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -5221,7 +5124,7 @@
       </c>
       <c r="C6" s="3"/>
     </row>
-    <row r="7" ht="51.75" spans="1:3">
+    <row r="7" ht="17.75" spans="1:3">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
@@ -5230,7 +5133,7 @@
       </c>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" ht="51.75" spans="1:3">
+    <row r="8" ht="17.75" spans="1:3">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -5239,7 +5142,7 @@
       </c>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" ht="51.75" spans="1:3">
+    <row r="9" ht="17.75" spans="1:3">
       <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
@@ -5248,7 +5151,7 @@
       </c>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" ht="51.75" spans="1:3">
+    <row r="10" ht="17.75" spans="1:3">
       <c r="A10" s="4" t="s">
         <v>5</v>
       </c>
@@ -5257,7 +5160,7 @@
       </c>
       <c r="C10" s="3"/>
     </row>
-    <row r="11" ht="51.75" spans="1:3">
+    <row r="11" ht="17.75" spans="1:3">
       <c r="A11" s="4" t="s">
         <v>5</v>
       </c>
@@ -5266,7 +5169,7 @@
       </c>
       <c r="C11" s="3"/>
     </row>
-    <row r="12" ht="51.75" spans="1:3">
+    <row r="12" ht="17.75" spans="1:3">
       <c r="A12" s="4" t="s">
         <v>5</v>
       </c>
@@ -5275,7 +5178,7 @@
       </c>
       <c r="C12" s="3"/>
     </row>
-    <row r="13" ht="51.75" spans="1:3">
+    <row r="13" ht="17.75" spans="1:3">
       <c r="A13" s="4" t="s">
         <v>5</v>
       </c>
@@ -5284,7 +5187,7 @@
       </c>
       <c r="C13" s="3"/>
     </row>
-    <row r="14" ht="51.75" spans="1:3">
+    <row r="14" ht="17.75" spans="1:3">
       <c r="A14" s="4" t="s">
         <v>5</v>
       </c>
@@ -5295,7 +5198,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" ht="51.75" spans="1:3">
+    <row r="15" ht="17.75" spans="1:3">
       <c r="A15" s="4" t="s">
         <v>5</v>
       </c>
@@ -5304,7 +5207,7 @@
       </c>
       <c r="C15" s="3"/>
     </row>
-    <row r="16" ht="51.75" spans="1:3">
+    <row r="16" ht="17.75" spans="1:3">
       <c r="A16" s="4" t="s">
         <v>5</v>
       </c>
@@ -5313,7 +5216,7 @@
       </c>
       <c r="C16" s="3"/>
     </row>
-    <row r="17" ht="51.75" spans="1:3">
+    <row r="17" ht="17.75" spans="1:3">
       <c r="A17" s="4" t="s">
         <v>5</v>
       </c>
@@ -5322,7 +5225,7 @@
       </c>
       <c r="C17" s="3"/>
     </row>
-    <row r="18" ht="51.75" spans="1:3">
+    <row r="18" ht="17.75" spans="1:3">
       <c r="A18" s="4" t="s">
         <v>5</v>
       </c>
@@ -5331,7 +5234,7 @@
       </c>
       <c r="C18" s="3"/>
     </row>
-    <row r="19" ht="51.75" spans="1:3">
+    <row r="19" ht="17.75" spans="1:3">
       <c r="A19" s="4" t="s">
         <v>5</v>
       </c>
@@ -5340,7 +5243,7 @@
       </c>
       <c r="C19" s="3"/>
     </row>
-    <row r="20" ht="51.75" spans="1:3">
+    <row r="20" ht="17.75" spans="1:3">
       <c r="A20" s="4" t="s">
         <v>5</v>
       </c>
@@ -5351,7 +5254,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" ht="51.75" spans="1:3">
+    <row r="21" ht="17.75" spans="1:3">
       <c r="A21" s="4" t="s">
         <v>5</v>
       </c>
@@ -5360,7 +5263,7 @@
       </c>
       <c r="C21" s="3"/>
     </row>
-    <row r="22" ht="51.75" spans="1:3">
+    <row r="22" ht="17.75" spans="1:3">
       <c r="A22" s="4" t="s">
         <v>5</v>
       </c>
@@ -5369,7 +5272,7 @@
       </c>
       <c r="C22" s="3"/>
     </row>
-    <row r="23" ht="51.75" spans="1:3">
+    <row r="23" ht="17.75" spans="1:3">
       <c r="A23" s="4" t="s">
         <v>5</v>
       </c>
@@ -5378,7 +5281,7 @@
       </c>
       <c r="C23" s="3"/>
     </row>
-    <row r="24" ht="51.75" spans="1:3">
+    <row r="24" ht="17.75" spans="1:3">
       <c r="A24" s="4" t="s">
         <v>5</v>
       </c>
@@ -5389,7 +5292,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" ht="51.75" spans="1:3">
+    <row r="25" ht="17.75" spans="1:3">
       <c r="A25" s="4" t="s">
         <v>5</v>
       </c>
@@ -5398,7 +5301,7 @@
       </c>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" ht="51.75" spans="1:3">
+    <row r="26" ht="17.75" spans="1:3">
       <c r="A26" s="4" t="s">
         <v>5</v>
       </c>
@@ -5407,7 +5310,7 @@
       </c>
       <c r="C26" s="3"/>
     </row>
-    <row r="27" ht="51.75" spans="1:3">
+    <row r="27" ht="17.75" spans="1:3">
       <c r="A27" s="4" t="s">
         <v>5</v>
       </c>
@@ -5416,7 +5319,7 @@
       </c>
       <c r="C27" s="3"/>
     </row>
-    <row r="28" ht="51.75" spans="1:3">
+    <row r="28" ht="17.75" spans="1:3">
       <c r="A28" s="4" t="s">
         <v>5</v>
       </c>
@@ -5465,7 +5368,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" ht="51.75" spans="1:3">
+    <row r="33" ht="17.75" spans="1:3">
       <c r="A33" s="2" t="s">
         <v>41</v>
       </c>
@@ -5474,7 +5377,7 @@
       </c>
       <c r="C33" s="3"/>
     </row>
-    <row r="34" ht="51.75" spans="1:3">
+    <row r="34" ht="17.75" spans="1:3">
       <c r="A34" s="2" t="s">
         <v>43</v>
       </c>
@@ -5483,7 +5386,7 @@
       </c>
       <c r="C34" s="3"/>
     </row>
-    <row r="35" ht="51.75" spans="1:3">
+    <row r="35" ht="17.75" spans="1:3">
       <c r="A35" s="2" t="s">
         <v>44</v>
       </c>
@@ -5575,7 +5478,7 @@
       </c>
       <c r="C44" s="3"/>
     </row>
-    <row r="45" ht="51.75" spans="1:3">
+    <row r="45" ht="17.75" spans="1:3">
       <c r="A45" s="4" t="s">
         <v>54</v>
       </c>
@@ -5584,7 +5487,7 @@
       </c>
       <c r="C45" s="3"/>
     </row>
-    <row r="46" ht="51.75" spans="1:3">
+    <row r="46" ht="17.75" spans="1:3">
       <c r="A46" s="4" t="s">
         <v>54</v>
       </c>
@@ -5593,7 +5496,7 @@
       </c>
       <c r="C46" s="3"/>
     </row>
-    <row r="47" ht="51.75" spans="1:3">
+    <row r="47" ht="17.75" spans="1:3">
       <c r="A47" s="4" t="s">
         <v>54</v>
       </c>
@@ -5602,7 +5505,7 @@
       </c>
       <c r="C47" s="3"/>
     </row>
-    <row r="48" ht="51.75" spans="1:3">
+    <row r="48" ht="17.75" spans="1:3">
       <c r="A48" s="4" t="s">
         <v>54</v>
       </c>
@@ -5611,7 +5514,7 @@
       </c>
       <c r="C48" s="3"/>
     </row>
-    <row r="49" ht="51.75" spans="1:3">
+    <row r="49" ht="17.75" spans="1:3">
       <c r="A49" s="4" t="s">
         <v>54</v>
       </c>
@@ -5620,7 +5523,7 @@
       </c>
       <c r="C49" s="3"/>
     </row>
-    <row r="50" ht="51.75" spans="1:3">
+    <row r="50" ht="17.75" spans="1:3">
       <c r="A50" s="4" t="s">
         <v>54</v>
       </c>
@@ -5629,7 +5532,7 @@
       </c>
       <c r="C50" s="3"/>
     </row>
-    <row r="51" ht="51.75" spans="1:3">
+    <row r="51" ht="17.75" spans="1:3">
       <c r="A51" s="4" t="s">
         <v>54</v>
       </c>
@@ -5638,7 +5541,7 @@
       </c>
       <c r="C51" s="3"/>
     </row>
-    <row r="52" ht="51.75" spans="1:3">
+    <row r="52" ht="17.75" spans="1:3">
       <c r="A52" s="4" t="s">
         <v>54</v>
       </c>
@@ -5647,7 +5550,7 @@
       </c>
       <c r="C52" s="3"/>
     </row>
-    <row r="53" ht="51.75" spans="1:3">
+    <row r="53" ht="17.75" spans="1:3">
       <c r="A53" s="4" t="s">
         <v>54</v>
       </c>
@@ -5656,7 +5559,7 @@
       </c>
       <c r="C53" s="3"/>
     </row>
-    <row r="54" ht="51.75" spans="1:3">
+    <row r="54" ht="17.75" spans="1:3">
       <c r="A54" s="4" t="s">
         <v>54</v>
       </c>
@@ -5667,7 +5570,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="55" ht="51.75" spans="1:3">
+    <row r="55" ht="17.75" spans="1:3">
       <c r="A55" s="4" t="s">
         <v>54</v>
       </c>
@@ -5676,7 +5579,7 @@
       </c>
       <c r="C55" s="3"/>
     </row>
-    <row r="56" ht="51.75" spans="1:3">
+    <row r="56" ht="17.75" spans="1:3">
       <c r="A56" s="4" t="s">
         <v>54</v>
       </c>
@@ -5685,7 +5588,7 @@
       </c>
       <c r="C56" s="3"/>
     </row>
-    <row r="57" ht="51.75" spans="1:3">
+    <row r="57" ht="17.75" spans="1:3">
       <c r="A57" s="4" t="s">
         <v>54</v>
       </c>
@@ -5694,7 +5597,7 @@
       </c>
       <c r="C57" s="3"/>
     </row>
-    <row r="58" ht="51.75" spans="1:3">
+    <row r="58" ht="17.75" spans="1:3">
       <c r="A58" s="4" t="s">
         <v>54</v>
       </c>
@@ -5703,7 +5606,7 @@
       </c>
       <c r="C58" s="3"/>
     </row>
-    <row r="59" ht="51.75" spans="1:3">
+    <row r="59" ht="17.75" spans="1:3">
       <c r="A59" s="4" t="s">
         <v>54</v>
       </c>
@@ -5712,7 +5615,7 @@
       </c>
       <c r="C59" s="3"/>
     </row>
-    <row r="60" ht="51.75" spans="1:3">
+    <row r="60" ht="17.75" spans="1:3">
       <c r="A60" s="4" t="s">
         <v>54</v>
       </c>
@@ -5721,7 +5624,7 @@
       </c>
       <c r="C60" s="3"/>
     </row>
-    <row r="61" ht="51.75" spans="1:3">
+    <row r="61" ht="17.75" spans="1:3">
       <c r="A61" s="4" t="s">
         <v>54</v>
       </c>
@@ -5730,7 +5633,7 @@
       </c>
       <c r="C61" s="3"/>
     </row>
-    <row r="62" ht="51.75" spans="1:3">
+    <row r="62" ht="17.75" spans="1:3">
       <c r="A62" s="2" t="s">
         <v>70</v>
       </c>
@@ -5748,7 +5651,7 @@
       </c>
       <c r="C63" s="3"/>
     </row>
-    <row r="64" ht="51.75" spans="1:3">
+    <row r="64" ht="17.75" spans="1:3">
       <c r="A64" s="4" t="s">
         <v>72</v>
       </c>
@@ -5757,7 +5660,7 @@
       </c>
       <c r="C64" s="3"/>
     </row>
-    <row r="65" ht="51.75" spans="1:3">
+    <row r="65" ht="17.75" spans="1:3">
       <c r="A65" s="4" t="s">
         <v>72</v>
       </c>
@@ -5766,7 +5669,7 @@
       </c>
       <c r="C65" s="3"/>
     </row>
-    <row r="66" ht="51.75" spans="1:3">
+    <row r="66" ht="17.75" spans="1:3">
       <c r="A66" s="4" t="s">
         <v>72</v>
       </c>
@@ -5784,7 +5687,7 @@
       </c>
       <c r="C67" s="3"/>
     </row>
-    <row r="68" ht="51.75" spans="1:3">
+    <row r="68" ht="17.75" spans="1:3">
       <c r="A68" s="6" t="s">
         <v>75</v>
       </c>
@@ -5793,7 +5696,7 @@
       </c>
       <c r="C68" s="3"/>
     </row>
-    <row r="69" ht="51.75" spans="1:3">
+    <row r="69" ht="17.75" spans="1:3">
       <c r="A69" s="6" t="s">
         <v>75</v>
       </c>
@@ -5802,7 +5705,7 @@
       </c>
       <c r="C69" s="3"/>
     </row>
-    <row r="70" ht="51.75" spans="1:3">
+    <row r="70" ht="17.75" spans="1:3">
       <c r="A70" s="6" t="s">
         <v>75</v>
       </c>
@@ -5813,7 +5716,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="71" ht="51.75" spans="1:3">
+    <row r="71" ht="17.75" spans="1:3">
       <c r="A71" s="6" t="s">
         <v>75</v>
       </c>
@@ -5822,7 +5725,7 @@
       </c>
       <c r="C71" s="3"/>
     </row>
-    <row r="72" ht="51.75" spans="1:3">
+    <row r="72" ht="17.75" spans="1:3">
       <c r="A72" s="6" t="s">
         <v>75</v>
       </c>
@@ -5831,7 +5734,7 @@
       </c>
       <c r="C72" s="3"/>
     </row>
-    <row r="73" ht="51.75" spans="1:3">
+    <row r="73" ht="17.75" spans="1:3">
       <c r="A73" s="6" t="s">
         <v>75</v>
       </c>
@@ -5840,7 +5743,7 @@
       </c>
       <c r="C73" s="3"/>
     </row>
-    <row r="74" ht="51.75" spans="1:3">
+    <row r="74" ht="17.75" spans="1:3">
       <c r="A74" s="4" t="s">
         <v>75</v>
       </c>
@@ -5860,7 +5763,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="76" ht="51.75" spans="1:3">
+    <row r="76" ht="17.75" spans="1:3">
       <c r="A76" s="6" t="s">
         <v>80</v>
       </c>
@@ -5869,7 +5772,7 @@
       </c>
       <c r="C76" s="3"/>
     </row>
-    <row r="77" ht="51.75" spans="1:3">
+    <row r="77" ht="17.75" spans="1:3">
       <c r="A77" s="6" t="s">
         <v>80</v>
       </c>
@@ -5878,7 +5781,7 @@
       </c>
       <c r="C77" s="3"/>
     </row>
-    <row r="78" ht="51.75" spans="1:3">
+    <row r="78" ht="17.75" spans="1:3">
       <c r="A78" s="6" t="s">
         <v>80</v>
       </c>
@@ -5887,7 +5790,7 @@
       </c>
       <c r="C78" s="3"/>
     </row>
-    <row r="79" ht="51.75" spans="1:3">
+    <row r="79" ht="17.75" spans="1:3">
       <c r="A79" s="6" t="s">
         <v>80</v>
       </c>
@@ -5896,7 +5799,7 @@
       </c>
       <c r="C79" s="3"/>
     </row>
-    <row r="80" ht="51.75" spans="1:3">
+    <row r="80" ht="17.75" spans="1:3">
       <c r="A80" s="6" t="s">
         <v>80</v>
       </c>
@@ -5905,7 +5808,7 @@
       </c>
       <c r="C80" s="3"/>
     </row>
-    <row r="81" ht="51.75" spans="1:3">
+    <row r="81" ht="17.75" spans="1:3">
       <c r="A81" s="6" t="s">
         <v>80</v>
       </c>
@@ -5914,7 +5817,7 @@
       </c>
       <c r="C81" s="3"/>
     </row>
-    <row r="82" ht="51.75" spans="1:3">
+    <row r="82" ht="17.75" spans="1:3">
       <c r="A82" s="6" t="s">
         <v>80</v>
       </c>
@@ -5923,7 +5826,7 @@
       </c>
       <c r="C82" s="3"/>
     </row>
-    <row r="83" ht="51.75" spans="1:3">
+    <row r="83" ht="17.75" spans="1:3">
       <c r="A83" s="6" t="s">
         <v>80</v>
       </c>
@@ -5932,7 +5835,7 @@
       </c>
       <c r="C83" s="3"/>
     </row>
-    <row r="84" ht="51.75" spans="1:3">
+    <row r="84" ht="17.75" spans="1:3">
       <c r="A84" s="6" t="s">
         <v>80</v>
       </c>
@@ -5941,7 +5844,7 @@
       </c>
       <c r="C84" s="3"/>
     </row>
-    <row r="85" ht="51.75" spans="1:3">
+    <row r="85" ht="17.75" spans="1:3">
       <c r="A85" s="4" t="s">
         <v>80</v>
       </c>
@@ -5950,7 +5853,7 @@
       </c>
       <c r="C85" s="3"/>
     </row>
-    <row r="86" ht="51.75" spans="1:3">
+    <row r="86" ht="17.75" spans="1:3">
       <c r="A86" s="2" t="s">
         <v>91</v>
       </c>
@@ -5959,7 +5862,7 @@
       </c>
       <c r="C86" s="3"/>
     </row>
-    <row r="87" ht="51.75" spans="1:3">
+    <row r="87" ht="17.75" spans="1:3">
       <c r="A87" s="2" t="s">
         <v>93</v>
       </c>
@@ -5968,7 +5871,7 @@
       </c>
       <c r="C87" s="3"/>
     </row>
-    <row r="88" ht="51.75" spans="1:3">
+    <row r="88" ht="17.75" spans="1:3">
       <c r="A88" s="2" t="s">
         <v>95</v>
       </c>
@@ -5977,7 +5880,7 @@
       </c>
       <c r="C88" s="3"/>
     </row>
-    <row r="89" ht="51.75" spans="1:3">
+    <row r="89" ht="17.75" spans="1:3">
       <c r="A89" s="2" t="s">
         <v>97</v>
       </c>
@@ -5995,7 +5898,7 @@
       </c>
       <c r="C90" s="3"/>
     </row>
-    <row r="91" ht="51.75" spans="1:3">
+    <row r="91" ht="34.75" spans="1:3">
       <c r="A91" s="4" t="s">
         <v>99</v>
       </c>
@@ -6004,7 +5907,7 @@
       </c>
       <c r="C91" s="3"/>
     </row>
-    <row r="92" ht="51.75" spans="1:3">
+    <row r="92" ht="34.75" spans="1:3">
       <c r="A92" s="4" t="s">
         <v>99</v>
       </c>
@@ -6013,7 +5916,7 @@
       </c>
       <c r="C92" s="3"/>
     </row>
-    <row r="93" ht="51.75" spans="1:3">
+    <row r="93" ht="34.75" spans="1:3">
       <c r="A93" s="4" t="s">
         <v>99</v>
       </c>
@@ -6031,7 +5934,7 @@
       </c>
       <c r="C94" s="3"/>
     </row>
-    <row r="95" ht="51.75" spans="1:3">
+    <row r="95" ht="17.75" spans="1:3">
       <c r="A95" s="4" t="s">
         <v>104</v>
       </c>
@@ -6049,7 +5952,7 @@
       </c>
       <c r="C96" s="3"/>
     </row>
-    <row r="97" ht="51.75" spans="1:3">
+    <row r="97" ht="17.75" spans="1:3">
       <c r="A97" s="4" t="s">
         <v>107</v>
       </c>
@@ -6058,7 +5961,7 @@
       </c>
       <c r="C97" s="3"/>
     </row>
-    <row r="98" ht="51.75" spans="1:3">
+    <row r="98" ht="17.75" spans="1:3">
       <c r="A98" s="2" t="s">
         <v>110</v>
       </c>
@@ -6067,7 +5970,7 @@
       </c>
       <c r="C98" s="3"/>
     </row>
-    <row r="99" ht="51.75" spans="1:3">
+    <row r="99" ht="17.75" spans="1:3">
       <c r="A99" s="2" t="s">
         <v>112</v>
       </c>
@@ -6089,7 +5992,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="101" ht="51.75" spans="1:3">
+    <row r="101" ht="34.75" spans="1:3">
       <c r="A101" s="4" t="s">
         <v>114</v>
       </c>
@@ -6098,7 +6001,7 @@
       </c>
       <c r="C101" s="3"/>
     </row>
-    <row r="102" ht="51.75" spans="1:3">
+    <row r="102" ht="34.75" spans="1:3">
       <c r="A102" s="4" t="s">
         <v>114</v>
       </c>
@@ -6107,7 +6010,7 @@
       </c>
       <c r="C102" s="3"/>
     </row>
-    <row r="103" ht="51.75" spans="1:3">
+    <row r="103" ht="34.75" spans="1:3">
       <c r="A103" s="4" t="s">
         <v>114</v>
       </c>
@@ -6116,7 +6019,7 @@
       </c>
       <c r="C103" s="3"/>
     </row>
-    <row r="104" ht="51.75" spans="1:3">
+    <row r="104" ht="34.75" spans="1:3">
       <c r="A104" s="4" t="s">
         <v>114</v>
       </c>
@@ -6134,7 +6037,7 @@
       </c>
       <c r="C105" s="3"/>
     </row>
-    <row r="106" ht="51.75" spans="1:3">
+    <row r="106" ht="17.75" spans="1:3">
       <c r="A106" s="4" t="s">
         <v>121</v>
       </c>
@@ -6143,7 +6046,7 @@
       </c>
       <c r="C106" s="3"/>
     </row>
-    <row r="107" ht="51.75" spans="1:3">
+    <row r="107" ht="17.75" spans="1:3">
       <c r="A107" s="4" t="s">
         <v>121</v>
       </c>
@@ -6152,7 +6055,7 @@
       </c>
       <c r="C107" s="3"/>
     </row>
-    <row r="108" ht="51.75" spans="1:3">
+    <row r="108" ht="17.75" spans="1:3">
       <c r="A108" s="4" t="s">
         <v>121</v>
       </c>
@@ -6161,7 +6064,7 @@
       </c>
       <c r="C108" s="3"/>
     </row>
-    <row r="109" ht="51.75" spans="1:3">
+    <row r="109" ht="17.75" spans="1:3">
       <c r="A109" s="4" t="s">
         <v>121</v>
       </c>
@@ -6170,7 +6073,7 @@
       </c>
       <c r="C109" s="3"/>
     </row>
-    <row r="110" ht="51.75" spans="1:3">
+    <row r="110" ht="17.75" spans="1:3">
       <c r="A110" s="4" t="s">
         <v>121</v>
       </c>
@@ -6188,7 +6091,7 @@
       </c>
       <c r="C111" s="3"/>
     </row>
-    <row r="112" ht="51.75" spans="1:3">
+    <row r="112" ht="17.75" spans="1:3">
       <c r="A112" s="4" t="s">
         <v>128</v>
       </c>
@@ -6206,7 +6109,7 @@
       </c>
       <c r="C113" s="3"/>
     </row>
-    <row r="114" ht="51.75" spans="1:3">
+    <row r="114" ht="17.75" spans="1:3">
       <c r="A114" s="6" t="s">
         <v>131</v>
       </c>
@@ -6215,7 +6118,7 @@
       </c>
       <c r="C114" s="3"/>
     </row>
-    <row r="115" ht="51.75" spans="1:3">
+    <row r="115" ht="17.75" spans="1:3">
       <c r="A115" s="6" t="s">
         <v>131</v>
       </c>
@@ -6224,7 +6127,7 @@
       </c>
       <c r="C115" s="3"/>
     </row>
-    <row r="116" ht="51.75" spans="1:3">
+    <row r="116" ht="17.75" spans="1:3">
       <c r="A116" s="6" t="s">
         <v>131</v>
       </c>
@@ -6233,7 +6136,7 @@
       </c>
       <c r="C116" s="3"/>
     </row>
-    <row r="117" ht="51.75" spans="1:3">
+    <row r="117" ht="17.75" spans="1:3">
       <c r="A117" s="6" t="s">
         <v>131</v>
       </c>
@@ -6242,7 +6145,7 @@
       </c>
       <c r="C117" s="3"/>
     </row>
-    <row r="118" ht="51.75" spans="1:3">
+    <row r="118" ht="17.75" spans="1:3">
       <c r="A118" s="6" t="s">
         <v>131</v>
       </c>
@@ -6251,7 +6154,7 @@
       </c>
       <c r="C118" s="3"/>
     </row>
-    <row r="119" ht="51.75" spans="1:3">
+    <row r="119" ht="17.75" spans="1:3">
       <c r="A119" s="6" t="s">
         <v>131</v>
       </c>
@@ -6260,7 +6163,7 @@
       </c>
       <c r="C119" s="3"/>
     </row>
-    <row r="120" ht="51.75" spans="1:3">
+    <row r="120" ht="17.75" spans="1:3">
       <c r="A120" s="6" t="s">
         <v>131</v>
       </c>
@@ -6269,7 +6172,7 @@
       </c>
       <c r="C120" s="3"/>
     </row>
-    <row r="121" ht="51.75" spans="1:3">
+    <row r="121" ht="17.75" spans="1:3">
       <c r="A121" s="6" t="s">
         <v>131</v>
       </c>
@@ -6278,7 +6181,7 @@
       </c>
       <c r="C121" s="3"/>
     </row>
-    <row r="122" ht="51.75" spans="1:3">
+    <row r="122" ht="17.75" spans="1:3">
       <c r="A122" s="6" t="s">
         <v>131</v>
       </c>
@@ -6287,7 +6190,7 @@
       </c>
       <c r="C122" s="3"/>
     </row>
-    <row r="123" ht="51.75" spans="1:3">
+    <row r="123" ht="17.75" spans="1:3">
       <c r="A123" s="6" t="s">
         <v>131</v>
       </c>
@@ -6296,7 +6199,7 @@
       </c>
       <c r="C123" s="3"/>
     </row>
-    <row r="124" ht="51.75" spans="1:3">
+    <row r="124" ht="17.75" spans="1:3">
       <c r="A124" s="6" t="s">
         <v>131</v>
       </c>
@@ -6305,7 +6208,7 @@
       </c>
       <c r="C124" s="3"/>
     </row>
-    <row r="125" ht="51.75" spans="1:3">
+    <row r="125" ht="17.75" spans="1:3">
       <c r="A125" s="6" t="s">
         <v>131</v>
       </c>
@@ -6314,7 +6217,7 @@
       </c>
       <c r="C125" s="3"/>
     </row>
-    <row r="126" ht="51.75" spans="1:3">
+    <row r="126" ht="17.75" spans="1:3">
       <c r="A126" s="6" t="s">
         <v>131</v>
       </c>
@@ -6323,7 +6226,7 @@
       </c>
       <c r="C126" s="3"/>
     </row>
-    <row r="127" ht="51.75" spans="1:3">
+    <row r="127" ht="17.75" spans="1:3">
       <c r="A127" s="6" t="s">
         <v>131</v>
       </c>
@@ -6332,7 +6235,7 @@
       </c>
       <c r="C127" s="3"/>
     </row>
-    <row r="128" ht="51.75" spans="1:3">
+    <row r="128" ht="17.75" spans="1:3">
       <c r="A128" s="6" t="s">
         <v>131</v>
       </c>
@@ -6341,7 +6244,7 @@
       </c>
       <c r="C128" s="3"/>
     </row>
-    <row r="129" ht="51.75" spans="1:3">
+    <row r="129" ht="17.75" spans="1:3">
       <c r="A129" s="6" t="s">
         <v>131</v>
       </c>
@@ -6350,7 +6253,7 @@
       </c>
       <c r="C129" s="3"/>
     </row>
-    <row r="130" ht="51.75" spans="1:3">
+    <row r="130" ht="17.75" spans="1:3">
       <c r="A130" s="6" t="s">
         <v>131</v>
       </c>
@@ -6359,7 +6262,7 @@
       </c>
       <c r="C130" s="3"/>
     </row>
-    <row r="131" ht="51.75" spans="1:3">
+    <row r="131" ht="17.75" spans="1:3">
       <c r="A131" s="6" t="s">
         <v>131</v>
       </c>
@@ -6368,7 +6271,7 @@
       </c>
       <c r="C131" s="3"/>
     </row>
-    <row r="132" ht="51.75" spans="1:3">
+    <row r="132" ht="17.75" spans="1:3">
       <c r="A132" s="6" t="s">
         <v>131</v>
       </c>
@@ -6377,7 +6280,7 @@
       </c>
       <c r="C132" s="3"/>
     </row>
-    <row r="133" ht="51.75" spans="1:3">
+    <row r="133" ht="17.75" spans="1:3">
       <c r="A133" s="6" t="s">
         <v>131</v>
       </c>
@@ -6386,7 +6289,7 @@
       </c>
       <c r="C133" s="3"/>
     </row>
-    <row r="134" ht="51.75" spans="1:3">
+    <row r="134" ht="17.75" spans="1:3">
       <c r="A134" s="6" t="s">
         <v>131</v>
       </c>
@@ -6395,7 +6298,7 @@
       </c>
       <c r="C134" s="3"/>
     </row>
-    <row r="135" ht="51.75" spans="1:3">
+    <row r="135" ht="17.75" spans="1:3">
       <c r="A135" s="6" t="s">
         <v>131</v>
       </c>
@@ -6404,7 +6307,7 @@
       </c>
       <c r="C135" s="3"/>
     </row>
-    <row r="136" ht="51.75" spans="1:3">
+    <row r="136" ht="17.75" spans="1:3">
       <c r="A136" s="6" t="s">
         <v>131</v>
       </c>
@@ -6413,7 +6316,7 @@
       </c>
       <c r="C136" s="3"/>
     </row>
-    <row r="137" ht="51.75" spans="1:3">
+    <row r="137" ht="17.75" spans="1:3">
       <c r="A137" s="6" t="s">
         <v>131</v>
       </c>
@@ -6422,7 +6325,7 @@
       </c>
       <c r="C137" s="3"/>
     </row>
-    <row r="138" ht="51.75" spans="1:3">
+    <row r="138" ht="17.75" spans="1:3">
       <c r="A138" s="6" t="s">
         <v>131</v>
       </c>
@@ -6431,7 +6334,7 @@
       </c>
       <c r="C138" s="3"/>
     </row>
-    <row r="139" ht="51.75" spans="1:3">
+    <row r="139" ht="17.75" spans="1:3">
       <c r="A139" s="6" t="s">
         <v>131</v>
       </c>
@@ -6440,7 +6343,7 @@
       </c>
       <c r="C139" s="3"/>
     </row>
-    <row r="140" ht="51.75" spans="1:3">
+    <row r="140" ht="17.75" spans="1:3">
       <c r="A140" s="6" t="s">
         <v>131</v>
       </c>
@@ -6449,7 +6352,7 @@
       </c>
       <c r="C140" s="3"/>
     </row>
-    <row r="141" ht="51.75" spans="1:3">
+    <row r="141" ht="17.75" spans="1:3">
       <c r="A141" s="6" t="s">
         <v>131</v>
       </c>
@@ -6458,7 +6361,7 @@
       </c>
       <c r="C141" s="3"/>
     </row>
-    <row r="142" ht="51.75" spans="1:3">
+    <row r="142" ht="17.75" spans="1:3">
       <c r="A142" s="6" t="s">
         <v>131</v>
       </c>
@@ -6467,7 +6370,7 @@
       </c>
       <c r="C142" s="3"/>
     </row>
-    <row r="143" ht="51.75" spans="1:3">
+    <row r="143" ht="17.75" spans="1:3">
       <c r="A143" s="6" t="s">
         <v>131</v>
       </c>
@@ -6478,7 +6381,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="144" ht="51.75" spans="1:3">
+    <row r="144" ht="17.75" spans="1:3">
       <c r="A144" s="6" t="s">
         <v>131</v>
       </c>
@@ -6487,7 +6390,7 @@
       </c>
       <c r="C144" s="3"/>
     </row>
-    <row r="145" ht="51.75" spans="1:3">
+    <row r="145" ht="17.75" spans="1:3">
       <c r="A145" s="6" t="s">
         <v>131</v>
       </c>
@@ -6496,7 +6399,7 @@
       </c>
       <c r="C145" s="3"/>
     </row>
-    <row r="146" ht="51.75" spans="1:3">
+    <row r="146" ht="17.75" spans="1:3">
       <c r="A146" s="6" t="s">
         <v>131</v>
       </c>
@@ -6505,7 +6408,7 @@
       </c>
       <c r="C146" s="3"/>
     </row>
-    <row r="147" ht="51.75" spans="1:3">
+    <row r="147" ht="17.75" spans="1:3">
       <c r="A147" s="6" t="s">
         <v>131</v>
       </c>
@@ -6516,7 +6419,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="148" ht="51.75" spans="1:3">
+    <row r="148" ht="17.75" spans="1:3">
       <c r="A148" s="6" t="s">
         <v>131</v>
       </c>
@@ -6525,7 +6428,7 @@
       </c>
       <c r="C148" s="3"/>
     </row>
-    <row r="149" ht="51.75" spans="1:3">
+    <row r="149" ht="17.75" spans="1:3">
       <c r="A149" s="4" t="s">
         <v>131</v>
       </c>
@@ -6543,7 +6446,7 @@
       </c>
       <c r="C150" s="3"/>
     </row>
-    <row r="151" ht="51.75" spans="1:3">
+    <row r="151" ht="17.75" spans="1:3">
       <c r="A151" s="4" t="s">
         <v>171</v>
       </c>
@@ -6552,7 +6455,7 @@
       </c>
       <c r="C151" s="3"/>
     </row>
-    <row r="152" ht="51.75" spans="1:3">
+    <row r="152" ht="17.75" spans="1:3">
       <c r="A152" s="4" t="s">
         <v>171</v>
       </c>
@@ -6561,7 +6464,7 @@
       </c>
       <c r="C152" s="3"/>
     </row>
-    <row r="153" ht="51.75" spans="1:3">
+    <row r="153" ht="17.75" spans="1:3">
       <c r="A153" s="4" t="s">
         <v>171</v>
       </c>
@@ -6572,7 +6475,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="154" ht="51.75" spans="1:3">
+    <row r="154" ht="17.75" spans="1:3">
       <c r="A154" s="4" t="s">
         <v>171</v>
       </c>
@@ -6581,7 +6484,7 @@
       </c>
       <c r="C154" s="3"/>
     </row>
-    <row r="155" ht="51.75" spans="1:3">
+    <row r="155" ht="17.75" spans="1:3">
       <c r="A155" s="4" t="s">
         <v>171</v>
       </c>
@@ -6590,7 +6493,7 @@
       </c>
       <c r="C155" s="3"/>
     </row>
-    <row r="156" ht="51.75" spans="1:3">
+    <row r="156" ht="17.75" spans="1:3">
       <c r="A156" s="4" t="s">
         <v>171</v>
       </c>
@@ -6598,6 +6501,17 @@
         <v>178</v>
       </c>
       <c r="C156" s="8"/>
+    </row>
+    <row r="157" spans="1:3">
+      <c r="A157">
+        <v>3</v>
+      </c>
+      <c r="B157">
+        <v>2</v>
+      </c>
+      <c r="C157">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
自动更新数据 - 2025-04-28 16:54:16
</commit_message>
<xml_diff>
--- a/data/raw/水晶.xlsx
+++ b/data/raw/水晶.xlsx
@@ -5055,10 +5055,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C157"/>
+  <dimension ref="A1:C156"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="119" topLeftCell="A149" workbookViewId="0">
-      <selection activeCell="B160" sqref="B160"/>
+    <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="119" topLeftCell="A150" workbookViewId="0">
+      <selection activeCell="C157" sqref="C157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelCol="2"/>
@@ -6502,17 +6502,6 @@
       </c>
       <c r="C156" s="8"/>
     </row>
-    <row r="157" spans="1:3">
-      <c r="A157">
-        <v>3</v>
-      </c>
-      <c r="B157">
-        <v>2</v>
-      </c>
-      <c r="C157">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
自动更新数据 - 2025-04-28 16:58:28
</commit_message>
<xml_diff>
--- a/data/raw/水晶.xlsx
+++ b/data/raw/水晶.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="181">
   <si>
     <t>名称</t>
   </si>
@@ -3823,6 +3823,12 @@
   </si>
   <si>
     <t>芙蓉石</t>
+  </si>
+  <si>
+    <t>段艳梅</t>
+  </si>
+  <si>
+    <t>卫金权</t>
   </si>
 </sst>
 </file>
@@ -5055,10 +5061,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C156"/>
+  <dimension ref="A1:C158"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="119" topLeftCell="A150" workbookViewId="0">
-      <selection activeCell="C157" sqref="C157"/>
+    <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="119" topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="A163" sqref="A163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelCol="2"/>
@@ -6502,6 +6508,17 @@
       </c>
       <c r="C156" s="8"/>
     </row>
+    <row r="158" spans="1:3">
+      <c r="A158">
+        <v>12344</v>
+      </c>
+      <c r="B158" t="s">
+        <v>179</v>
+      </c>
+      <c r="C158" t="s">
+        <v>180</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
自动更新数据 - 2025-04-28 18:29:00
</commit_message>
<xml_diff>
--- a/data/raw/水晶.xlsx
+++ b/data/raw/水晶.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="179">
   <si>
     <t>名称</t>
   </si>
@@ -3823,12 +3823,6 @@
   </si>
   <si>
     <t>芙蓉石</t>
-  </si>
-  <si>
-    <t>段艳梅</t>
-  </si>
-  <si>
-    <t>卫金权</t>
   </si>
 </sst>
 </file>
@@ -4213,49 +4207,10 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="9">
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -4384,7 +4339,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -4396,34 +4351,34 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -4508,32 +4463,29 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -5061,10 +5013,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C158"/>
+  <dimension ref="A1:C156"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="119" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="A163" sqref="A163"/>
+    <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="119" workbookViewId="0">
+      <selection activeCell="A159" sqref="$A1:$XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelCol="2"/>
@@ -5074,7 +5026,7 @@
     <col min="3" max="3" width="40.1538461538462" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="17.75" spans="1:3">
+    <row r="1" ht="17" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5085,7 +5037,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" ht="17.75" spans="1:3">
+    <row r="2" ht="17" spans="1:3">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -5103,7 +5055,7 @@
       </c>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" ht="17.75" spans="1:3">
+    <row r="4" ht="17" spans="1:3">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -5112,7 +5064,7 @@
       </c>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" ht="17.75" spans="1:3">
+    <row r="5" ht="17" spans="1:3">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -5121,7 +5073,7 @@
       </c>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" ht="17.75" spans="1:3">
+    <row r="6" ht="17" spans="1:3">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -5130,7 +5082,7 @@
       </c>
       <c r="C6" s="3"/>
     </row>
-    <row r="7" ht="17.75" spans="1:3">
+    <row r="7" ht="17" spans="1:3">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
@@ -5139,7 +5091,7 @@
       </c>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" ht="17.75" spans="1:3">
+    <row r="8" ht="17" spans="1:3">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -5148,7 +5100,7 @@
       </c>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" ht="17.75" spans="1:3">
+    <row r="9" ht="17" spans="1:3">
       <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
@@ -5157,7 +5109,7 @@
       </c>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" ht="17.75" spans="1:3">
+    <row r="10" ht="17" spans="1:3">
       <c r="A10" s="4" t="s">
         <v>5</v>
       </c>
@@ -5166,7 +5118,7 @@
       </c>
       <c r="C10" s="3"/>
     </row>
-    <row r="11" ht="17.75" spans="1:3">
+    <row r="11" ht="17" spans="1:3">
       <c r="A11" s="4" t="s">
         <v>5</v>
       </c>
@@ -5175,7 +5127,7 @@
       </c>
       <c r="C11" s="3"/>
     </row>
-    <row r="12" ht="17.75" spans="1:3">
+    <row r="12" ht="17" spans="1:3">
       <c r="A12" s="4" t="s">
         <v>5</v>
       </c>
@@ -5184,7 +5136,7 @@
       </c>
       <c r="C12" s="3"/>
     </row>
-    <row r="13" ht="17.75" spans="1:3">
+    <row r="13" ht="17" spans="1:3">
       <c r="A13" s="4" t="s">
         <v>5</v>
       </c>
@@ -5193,7 +5145,7 @@
       </c>
       <c r="C13" s="3"/>
     </row>
-    <row r="14" ht="17.75" spans="1:3">
+    <row r="14" ht="17" spans="1:3">
       <c r="A14" s="4" t="s">
         <v>5</v>
       </c>
@@ -5204,7 +5156,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" ht="17.75" spans="1:3">
+    <row r="15" ht="17" spans="1:3">
       <c r="A15" s="4" t="s">
         <v>5</v>
       </c>
@@ -5213,7 +5165,7 @@
       </c>
       <c r="C15" s="3"/>
     </row>
-    <row r="16" ht="17.75" spans="1:3">
+    <row r="16" ht="17" spans="1:3">
       <c r="A16" s="4" t="s">
         <v>5</v>
       </c>
@@ -5222,7 +5174,7 @@
       </c>
       <c r="C16" s="3"/>
     </row>
-    <row r="17" ht="17.75" spans="1:3">
+    <row r="17" ht="17" spans="1:3">
       <c r="A17" s="4" t="s">
         <v>5</v>
       </c>
@@ -5231,7 +5183,7 @@
       </c>
       <c r="C17" s="3"/>
     </row>
-    <row r="18" ht="17.75" spans="1:3">
+    <row r="18" ht="17" spans="1:3">
       <c r="A18" s="4" t="s">
         <v>5</v>
       </c>
@@ -5240,7 +5192,7 @@
       </c>
       <c r="C18" s="3"/>
     </row>
-    <row r="19" ht="17.75" spans="1:3">
+    <row r="19" ht="17" spans="1:3">
       <c r="A19" s="4" t="s">
         <v>5</v>
       </c>
@@ -5249,7 +5201,7 @@
       </c>
       <c r="C19" s="3"/>
     </row>
-    <row r="20" ht="17.75" spans="1:3">
+    <row r="20" ht="17" spans="1:3">
       <c r="A20" s="4" t="s">
         <v>5</v>
       </c>
@@ -5260,7 +5212,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" ht="17.75" spans="1:3">
+    <row r="21" ht="17" spans="1:3">
       <c r="A21" s="4" t="s">
         <v>5</v>
       </c>
@@ -5269,7 +5221,7 @@
       </c>
       <c r="C21" s="3"/>
     </row>
-    <row r="22" ht="17.75" spans="1:3">
+    <row r="22" ht="17" spans="1:3">
       <c r="A22" s="4" t="s">
         <v>5</v>
       </c>
@@ -5278,7 +5230,7 @@
       </c>
       <c r="C22" s="3"/>
     </row>
-    <row r="23" ht="17.75" spans="1:3">
+    <row r="23" ht="17" spans="1:3">
       <c r="A23" s="4" t="s">
         <v>5</v>
       </c>
@@ -5287,7 +5239,7 @@
       </c>
       <c r="C23" s="3"/>
     </row>
-    <row r="24" ht="17.75" spans="1:3">
+    <row r="24" ht="17" spans="1:3">
       <c r="A24" s="4" t="s">
         <v>5</v>
       </c>
@@ -5298,7 +5250,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" ht="17.75" spans="1:3">
+    <row r="25" ht="17" spans="1:3">
       <c r="A25" s="4" t="s">
         <v>5</v>
       </c>
@@ -5307,7 +5259,7 @@
       </c>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" ht="17.75" spans="1:3">
+    <row r="26" ht="17" spans="1:3">
       <c r="A26" s="4" t="s">
         <v>5</v>
       </c>
@@ -5316,7 +5268,7 @@
       </c>
       <c r="C26" s="3"/>
     </row>
-    <row r="27" ht="17.75" spans="1:3">
+    <row r="27" ht="17" spans="1:3">
       <c r="A27" s="4" t="s">
         <v>5</v>
       </c>
@@ -5325,7 +5277,7 @@
       </c>
       <c r="C27" s="3"/>
     </row>
-    <row r="28" ht="17.75" spans="1:3">
+    <row r="28" ht="17" spans="1:3">
       <c r="A28" s="4" t="s">
         <v>5</v>
       </c>
@@ -5334,7 +5286,7 @@
       </c>
       <c r="C28" s="3"/>
     </row>
-    <row r="29" ht="17.75" spans="1:3">
+    <row r="29" ht="17" spans="1:3">
       <c r="A29" s="2" t="s">
         <v>35</v>
       </c>
@@ -5354,7 +5306,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="31" ht="17.75" spans="1:3">
+    <row r="31" ht="17" spans="1:3">
       <c r="A31" s="4" t="s">
         <v>36</v>
       </c>
@@ -5363,7 +5315,7 @@
       </c>
       <c r="C31" s="3"/>
     </row>
-    <row r="32" ht="17.75" spans="1:3">
+    <row r="32" ht="17" spans="1:3">
       <c r="A32" s="2" t="s">
         <v>39</v>
       </c>
@@ -5374,7 +5326,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" ht="17.75" spans="1:3">
+    <row r="33" ht="17" spans="1:3">
       <c r="A33" s="2" t="s">
         <v>41</v>
       </c>
@@ -5383,7 +5335,7 @@
       </c>
       <c r="C33" s="3"/>
     </row>
-    <row r="34" ht="17.75" spans="1:3">
+    <row r="34" ht="17" spans="1:3">
       <c r="A34" s="2" t="s">
         <v>43</v>
       </c>
@@ -5392,7 +5344,7 @@
       </c>
       <c r="C34" s="3"/>
     </row>
-    <row r="35" ht="17.75" spans="1:3">
+    <row r="35" ht="17" spans="1:3">
       <c r="A35" s="2" t="s">
         <v>44</v>
       </c>
@@ -5401,7 +5353,7 @@
       </c>
       <c r="C35" s="3"/>
     </row>
-    <row r="36" ht="17.75" spans="1:3">
+    <row r="36" ht="17" spans="1:3">
       <c r="A36" s="2" t="s">
         <v>45</v>
       </c>
@@ -5421,7 +5373,7 @@
       </c>
       <c r="C37" s="3"/>
     </row>
-    <row r="38" ht="17.75" spans="1:3">
+    <row r="38" ht="17" spans="1:3">
       <c r="A38" s="4" t="s">
         <v>47</v>
       </c>
@@ -5430,7 +5382,7 @@
       </c>
       <c r="C38" s="3"/>
     </row>
-    <row r="39" ht="17.75" spans="1:3">
+    <row r="39" ht="17" spans="1:3">
       <c r="A39" s="4" t="s">
         <v>47</v>
       </c>
@@ -5439,7 +5391,7 @@
       </c>
       <c r="C39" s="3"/>
     </row>
-    <row r="40" ht="17.75" spans="1:3">
+    <row r="40" ht="17" spans="1:3">
       <c r="A40" s="4" t="s">
         <v>47</v>
       </c>
@@ -5448,7 +5400,7 @@
       </c>
       <c r="C40" s="3"/>
     </row>
-    <row r="41" ht="17.75" spans="1:3">
+    <row r="41" ht="17" spans="1:3">
       <c r="A41" s="4" t="s">
         <v>47</v>
       </c>
@@ -5457,7 +5409,7 @@
       </c>
       <c r="C41" s="3"/>
     </row>
-    <row r="42" ht="17.75" spans="1:3">
+    <row r="42" ht="17" spans="1:3">
       <c r="A42" s="4" t="s">
         <v>47</v>
       </c>
@@ -5466,7 +5418,7 @@
       </c>
       <c r="C42" s="3"/>
     </row>
-    <row r="43" ht="17.75" spans="1:3">
+    <row r="43" ht="17" spans="1:3">
       <c r="A43" s="2" t="s">
         <v>53</v>
       </c>
@@ -5484,7 +5436,7 @@
       </c>
       <c r="C44" s="3"/>
     </row>
-    <row r="45" ht="17.75" spans="1:3">
+    <row r="45" ht="17" spans="1:3">
       <c r="A45" s="4" t="s">
         <v>54</v>
       </c>
@@ -5493,7 +5445,7 @@
       </c>
       <c r="C45" s="3"/>
     </row>
-    <row r="46" ht="17.75" spans="1:3">
+    <row r="46" ht="17" spans="1:3">
       <c r="A46" s="4" t="s">
         <v>54</v>
       </c>
@@ -5502,7 +5454,7 @@
       </c>
       <c r="C46" s="3"/>
     </row>
-    <row r="47" ht="17.75" spans="1:3">
+    <row r="47" ht="17" spans="1:3">
       <c r="A47" s="4" t="s">
         <v>54</v>
       </c>
@@ -5511,7 +5463,7 @@
       </c>
       <c r="C47" s="3"/>
     </row>
-    <row r="48" ht="17.75" spans="1:3">
+    <row r="48" ht="17" spans="1:3">
       <c r="A48" s="4" t="s">
         <v>54</v>
       </c>
@@ -5520,7 +5472,7 @@
       </c>
       <c r="C48" s="3"/>
     </row>
-    <row r="49" ht="17.75" spans="1:3">
+    <row r="49" ht="17" spans="1:3">
       <c r="A49" s="4" t="s">
         <v>54</v>
       </c>
@@ -5529,7 +5481,7 @@
       </c>
       <c r="C49" s="3"/>
     </row>
-    <row r="50" ht="17.75" spans="1:3">
+    <row r="50" ht="17" spans="1:3">
       <c r="A50" s="4" t="s">
         <v>54</v>
       </c>
@@ -5538,7 +5490,7 @@
       </c>
       <c r="C50" s="3"/>
     </row>
-    <row r="51" ht="17.75" spans="1:3">
+    <row r="51" ht="17" spans="1:3">
       <c r="A51" s="4" t="s">
         <v>54</v>
       </c>
@@ -5547,7 +5499,7 @@
       </c>
       <c r="C51" s="3"/>
     </row>
-    <row r="52" ht="17.75" spans="1:3">
+    <row r="52" ht="17" spans="1:3">
       <c r="A52" s="4" t="s">
         <v>54</v>
       </c>
@@ -5556,7 +5508,7 @@
       </c>
       <c r="C52" s="3"/>
     </row>
-    <row r="53" ht="17.75" spans="1:3">
+    <row r="53" ht="17" spans="1:3">
       <c r="A53" s="4" t="s">
         <v>54</v>
       </c>
@@ -5565,7 +5517,7 @@
       </c>
       <c r="C53" s="3"/>
     </row>
-    <row r="54" ht="17.75" spans="1:3">
+    <row r="54" ht="17" spans="1:3">
       <c r="A54" s="4" t="s">
         <v>54</v>
       </c>
@@ -5576,7 +5528,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="55" ht="17.75" spans="1:3">
+    <row r="55" ht="17" spans="1:3">
       <c r="A55" s="4" t="s">
         <v>54</v>
       </c>
@@ -5585,7 +5537,7 @@
       </c>
       <c r="C55" s="3"/>
     </row>
-    <row r="56" ht="17.75" spans="1:3">
+    <row r="56" ht="17" spans="1:3">
       <c r="A56" s="4" t="s">
         <v>54</v>
       </c>
@@ -5594,7 +5546,7 @@
       </c>
       <c r="C56" s="3"/>
     </row>
-    <row r="57" ht="17.75" spans="1:3">
+    <row r="57" ht="17" spans="1:3">
       <c r="A57" s="4" t="s">
         <v>54</v>
       </c>
@@ -5603,7 +5555,7 @@
       </c>
       <c r="C57" s="3"/>
     </row>
-    <row r="58" ht="17.75" spans="1:3">
+    <row r="58" ht="17" spans="1:3">
       <c r="A58" s="4" t="s">
         <v>54</v>
       </c>
@@ -5612,7 +5564,7 @@
       </c>
       <c r="C58" s="3"/>
     </row>
-    <row r="59" ht="17.75" spans="1:3">
+    <row r="59" ht="17" spans="1:3">
       <c r="A59" s="4" t="s">
         <v>54</v>
       </c>
@@ -5621,7 +5573,7 @@
       </c>
       <c r="C59" s="3"/>
     </row>
-    <row r="60" ht="17.75" spans="1:3">
+    <row r="60" ht="17" spans="1:3">
       <c r="A60" s="4" t="s">
         <v>54</v>
       </c>
@@ -5630,7 +5582,7 @@
       </c>
       <c r="C60" s="3"/>
     </row>
-    <row r="61" ht="17.75" spans="1:3">
+    <row r="61" ht="17" spans="1:3">
       <c r="A61" s="4" t="s">
         <v>54</v>
       </c>
@@ -5639,7 +5591,7 @@
       </c>
       <c r="C61" s="3"/>
     </row>
-    <row r="62" ht="17.75" spans="1:3">
+    <row r="62" ht="17" spans="1:3">
       <c r="A62" s="2" t="s">
         <v>70</v>
       </c>
@@ -5657,7 +5609,7 @@
       </c>
       <c r="C63" s="3"/>
     </row>
-    <row r="64" ht="17.75" spans="1:3">
+    <row r="64" ht="17" spans="1:3">
       <c r="A64" s="4" t="s">
         <v>72</v>
       </c>
@@ -5666,7 +5618,7 @@
       </c>
       <c r="C64" s="3"/>
     </row>
-    <row r="65" ht="17.75" spans="1:3">
+    <row r="65" ht="17" spans="1:3">
       <c r="A65" s="4" t="s">
         <v>72</v>
       </c>
@@ -5675,7 +5627,7 @@
       </c>
       <c r="C65" s="3"/>
     </row>
-    <row r="66" ht="17.75" spans="1:3">
+    <row r="66" ht="17" spans="1:3">
       <c r="A66" s="4" t="s">
         <v>72</v>
       </c>
@@ -5685,7 +5637,7 @@
       <c r="C66" s="3"/>
     </row>
     <row r="67" ht="18.5" customHeight="1" spans="1:3">
-      <c r="A67" s="6" t="s">
+      <c r="A67" s="4" t="s">
         <v>75</v>
       </c>
       <c r="B67" s="2" t="s">
@@ -5693,8 +5645,8 @@
       </c>
       <c r="C67" s="3"/>
     </row>
-    <row r="68" ht="17.75" spans="1:3">
-      <c r="A68" s="6" t="s">
+    <row r="68" ht="17" spans="1:3">
+      <c r="A68" s="4" t="s">
         <v>75</v>
       </c>
       <c r="B68" s="2" t="s">
@@ -5702,8 +5654,8 @@
       </c>
       <c r="C68" s="3"/>
     </row>
-    <row r="69" ht="17.75" spans="1:3">
-      <c r="A69" s="6" t="s">
+    <row r="69" ht="17" spans="1:3">
+      <c r="A69" s="4" t="s">
         <v>75</v>
       </c>
       <c r="B69" s="2" t="s">
@@ -5711,8 +5663,8 @@
       </c>
       <c r="C69" s="3"/>
     </row>
-    <row r="70" ht="17.75" spans="1:3">
-      <c r="A70" s="6" t="s">
+    <row r="70" ht="17" spans="1:3">
+      <c r="A70" s="4" t="s">
         <v>75</v>
       </c>
       <c r="B70" s="2" t="s">
@@ -5722,8 +5674,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="71" ht="17.75" spans="1:3">
-      <c r="A71" s="6" t="s">
+    <row r="71" ht="17" spans="1:3">
+      <c r="A71" s="4" t="s">
         <v>75</v>
       </c>
       <c r="B71" s="2" t="s">
@@ -5731,8 +5683,8 @@
       </c>
       <c r="C71" s="3"/>
     </row>
-    <row r="72" ht="17.75" spans="1:3">
-      <c r="A72" s="6" t="s">
+    <row r="72" ht="17" spans="1:3">
+      <c r="A72" s="4" t="s">
         <v>75</v>
       </c>
       <c r="B72" s="2" t="s">
@@ -5740,8 +5692,8 @@
       </c>
       <c r="C72" s="3"/>
     </row>
-    <row r="73" ht="17.75" spans="1:3">
-      <c r="A73" s="6" t="s">
+    <row r="73" ht="17" spans="1:3">
+      <c r="A73" s="4" t="s">
         <v>75</v>
       </c>
       <c r="B73" s="2" t="s">
@@ -5749,7 +5701,7 @@
       </c>
       <c r="C73" s="3"/>
     </row>
-    <row r="74" ht="17.75" spans="1:3">
+    <row r="74" ht="17" spans="1:3">
       <c r="A74" s="4" t="s">
         <v>75</v>
       </c>
@@ -5759,7 +5711,7 @@
       <c r="C74" s="3"/>
     </row>
     <row r="75" ht="56" customHeight="1" spans="1:3">
-      <c r="A75" s="6" t="s">
+      <c r="A75" s="4" t="s">
         <v>78</v>
       </c>
       <c r="B75" s="2" t="s">
@@ -5769,8 +5721,8 @@
         <v>79</v>
       </c>
     </row>
-    <row r="76" ht="17.75" spans="1:3">
-      <c r="A76" s="6" t="s">
+    <row r="76" ht="17" spans="1:3">
+      <c r="A76" s="4" t="s">
         <v>80</v>
       </c>
       <c r="B76" s="2" t="s">
@@ -5778,8 +5730,8 @@
       </c>
       <c r="C76" s="3"/>
     </row>
-    <row r="77" ht="17.75" spans="1:3">
-      <c r="A77" s="6" t="s">
+    <row r="77" ht="17" spans="1:3">
+      <c r="A77" s="4" t="s">
         <v>80</v>
       </c>
       <c r="B77" s="2" t="s">
@@ -5787,8 +5739,8 @@
       </c>
       <c r="C77" s="3"/>
     </row>
-    <row r="78" ht="17.75" spans="1:3">
-      <c r="A78" s="6" t="s">
+    <row r="78" ht="17" spans="1:3">
+      <c r="A78" s="4" t="s">
         <v>80</v>
       </c>
       <c r="B78" s="2" t="s">
@@ -5796,8 +5748,8 @@
       </c>
       <c r="C78" s="3"/>
     </row>
-    <row r="79" ht="17.75" spans="1:3">
-      <c r="A79" s="6" t="s">
+    <row r="79" ht="17" spans="1:3">
+      <c r="A79" s="4" t="s">
         <v>80</v>
       </c>
       <c r="B79" s="2" t="s">
@@ -5805,8 +5757,8 @@
       </c>
       <c r="C79" s="3"/>
     </row>
-    <row r="80" ht="17.75" spans="1:3">
-      <c r="A80" s="6" t="s">
+    <row r="80" ht="17" spans="1:3">
+      <c r="A80" s="4" t="s">
         <v>80</v>
       </c>
       <c r="B80" s="2" t="s">
@@ -5814,8 +5766,8 @@
       </c>
       <c r="C80" s="3"/>
     </row>
-    <row r="81" ht="17.75" spans="1:3">
-      <c r="A81" s="6" t="s">
+    <row r="81" ht="17" spans="1:3">
+      <c r="A81" s="4" t="s">
         <v>80</v>
       </c>
       <c r="B81" s="2" t="s">
@@ -5823,8 +5775,8 @@
       </c>
       <c r="C81" s="3"/>
     </row>
-    <row r="82" ht="17.75" spans="1:3">
-      <c r="A82" s="6" t="s">
+    <row r="82" ht="17" spans="1:3">
+      <c r="A82" s="4" t="s">
         <v>80</v>
       </c>
       <c r="B82" s="2" t="s">
@@ -5832,8 +5784,8 @@
       </c>
       <c r="C82" s="3"/>
     </row>
-    <row r="83" ht="17.75" spans="1:3">
-      <c r="A83" s="6" t="s">
+    <row r="83" ht="17" spans="1:3">
+      <c r="A83" s="4" t="s">
         <v>80</v>
       </c>
       <c r="B83" s="2" t="s">
@@ -5841,8 +5793,8 @@
       </c>
       <c r="C83" s="3"/>
     </row>
-    <row r="84" ht="17.75" spans="1:3">
-      <c r="A84" s="6" t="s">
+    <row r="84" ht="17" spans="1:3">
+      <c r="A84" s="4" t="s">
         <v>80</v>
       </c>
       <c r="B84" s="2" t="s">
@@ -5850,7 +5802,7 @@
       </c>
       <c r="C84" s="3"/>
     </row>
-    <row r="85" ht="17.75" spans="1:3">
+    <row r="85" ht="17" spans="1:3">
       <c r="A85" s="4" t="s">
         <v>80</v>
       </c>
@@ -5859,7 +5811,7 @@
       </c>
       <c r="C85" s="3"/>
     </row>
-    <row r="86" ht="17.75" spans="1:3">
+    <row r="86" ht="17" spans="1:3">
       <c r="A86" s="2" t="s">
         <v>91</v>
       </c>
@@ -5868,7 +5820,7 @@
       </c>
       <c r="C86" s="3"/>
     </row>
-    <row r="87" ht="17.75" spans="1:3">
+    <row r="87" ht="17" spans="1:3">
       <c r="A87" s="2" t="s">
         <v>93</v>
       </c>
@@ -5877,7 +5829,7 @@
       </c>
       <c r="C87" s="3"/>
     </row>
-    <row r="88" ht="17.75" spans="1:3">
+    <row r="88" ht="17" spans="1:3">
       <c r="A88" s="2" t="s">
         <v>95</v>
       </c>
@@ -5886,7 +5838,7 @@
       </c>
       <c r="C88" s="3"/>
     </row>
-    <row r="89" ht="17.75" spans="1:3">
+    <row r="89" ht="17" spans="1:3">
       <c r="A89" s="2" t="s">
         <v>97</v>
       </c>
@@ -5904,7 +5856,7 @@
       </c>
       <c r="C90" s="3"/>
     </row>
-    <row r="91" ht="34.75" spans="1:3">
+    <row r="91" ht="34" spans="1:3">
       <c r="A91" s="4" t="s">
         <v>99</v>
       </c>
@@ -5913,7 +5865,7 @@
       </c>
       <c r="C91" s="3"/>
     </row>
-    <row r="92" ht="34.75" spans="1:3">
+    <row r="92" ht="34" spans="1:3">
       <c r="A92" s="4" t="s">
         <v>99</v>
       </c>
@@ -5922,7 +5874,7 @@
       </c>
       <c r="C92" s="3"/>
     </row>
-    <row r="93" ht="34.75" spans="1:3">
+    <row r="93" ht="34" spans="1:3">
       <c r="A93" s="4" t="s">
         <v>99</v>
       </c>
@@ -5940,7 +5892,7 @@
       </c>
       <c r="C94" s="3"/>
     </row>
-    <row r="95" ht="17.75" spans="1:3">
+    <row r="95" ht="17" spans="1:3">
       <c r="A95" s="4" t="s">
         <v>104</v>
       </c>
@@ -5958,7 +5910,7 @@
       </c>
       <c r="C96" s="3"/>
     </row>
-    <row r="97" ht="17.75" spans="1:3">
+    <row r="97" ht="17" spans="1:3">
       <c r="A97" s="4" t="s">
         <v>107</v>
       </c>
@@ -5967,7 +5919,7 @@
       </c>
       <c r="C97" s="3"/>
     </row>
-    <row r="98" ht="17.75" spans="1:3">
+    <row r="98" ht="17" spans="1:3">
       <c r="A98" s="2" t="s">
         <v>110</v>
       </c>
@@ -5976,7 +5928,7 @@
       </c>
       <c r="C98" s="3"/>
     </row>
-    <row r="99" ht="17.75" spans="1:3">
+    <row r="99" ht="17" spans="1:3">
       <c r="A99" s="2" t="s">
         <v>112</v>
       </c>
@@ -5994,11 +5946,11 @@
       <c r="B100" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C100" s="7" t="s">
+      <c r="C100" s="6" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="101" ht="34.75" spans="1:3">
+    <row r="101" ht="34" spans="1:3">
       <c r="A101" s="4" t="s">
         <v>114</v>
       </c>
@@ -6007,7 +5959,7 @@
       </c>
       <c r="C101" s="3"/>
     </row>
-    <row r="102" ht="34.75" spans="1:3">
+    <row r="102" ht="34" spans="1:3">
       <c r="A102" s="4" t="s">
         <v>114</v>
       </c>
@@ -6016,7 +5968,7 @@
       </c>
       <c r="C102" s="3"/>
     </row>
-    <row r="103" ht="34.75" spans="1:3">
+    <row r="103" ht="34" spans="1:3">
       <c r="A103" s="4" t="s">
         <v>114</v>
       </c>
@@ -6025,7 +5977,7 @@
       </c>
       <c r="C103" s="3"/>
     </row>
-    <row r="104" ht="34.75" spans="1:3">
+    <row r="104" ht="34" spans="1:3">
       <c r="A104" s="4" t="s">
         <v>114</v>
       </c>
@@ -6043,7 +5995,7 @@
       </c>
       <c r="C105" s="3"/>
     </row>
-    <row r="106" ht="17.75" spans="1:3">
+    <row r="106" ht="17" spans="1:3">
       <c r="A106" s="4" t="s">
         <v>121</v>
       </c>
@@ -6052,7 +6004,7 @@
       </c>
       <c r="C106" s="3"/>
     </row>
-    <row r="107" ht="17.75" spans="1:3">
+    <row r="107" ht="17" spans="1:3">
       <c r="A107" s="4" t="s">
         <v>121</v>
       </c>
@@ -6061,7 +6013,7 @@
       </c>
       <c r="C107" s="3"/>
     </row>
-    <row r="108" ht="17.75" spans="1:3">
+    <row r="108" ht="17" spans="1:3">
       <c r="A108" s="4" t="s">
         <v>121</v>
       </c>
@@ -6070,7 +6022,7 @@
       </c>
       <c r="C108" s="3"/>
     </row>
-    <row r="109" ht="17.75" spans="1:3">
+    <row r="109" ht="17" spans="1:3">
       <c r="A109" s="4" t="s">
         <v>121</v>
       </c>
@@ -6079,7 +6031,7 @@
       </c>
       <c r="C109" s="3"/>
     </row>
-    <row r="110" ht="17.75" spans="1:3">
+    <row r="110" ht="17" spans="1:3">
       <c r="A110" s="4" t="s">
         <v>121</v>
       </c>
@@ -6097,7 +6049,7 @@
       </c>
       <c r="C111" s="3"/>
     </row>
-    <row r="112" ht="17.75" spans="1:3">
+    <row r="112" ht="17" spans="1:3">
       <c r="A112" s="4" t="s">
         <v>128</v>
       </c>
@@ -6107,7 +6059,7 @@
       <c r="C112" s="3"/>
     </row>
     <row r="113" ht="69.5" customHeight="1" spans="1:3">
-      <c r="A113" s="6" t="s">
+      <c r="A113" s="4" t="s">
         <v>131</v>
       </c>
       <c r="B113" s="2" t="s">
@@ -6115,8 +6067,8 @@
       </c>
       <c r="C113" s="3"/>
     </row>
-    <row r="114" ht="17.75" spans="1:3">
-      <c r="A114" s="6" t="s">
+    <row r="114" ht="17" spans="1:3">
+      <c r="A114" s="4" t="s">
         <v>131</v>
       </c>
       <c r="B114" s="2" t="s">
@@ -6124,8 +6076,8 @@
       </c>
       <c r="C114" s="3"/>
     </row>
-    <row r="115" ht="17.75" spans="1:3">
-      <c r="A115" s="6" t="s">
+    <row r="115" ht="17" spans="1:3">
+      <c r="A115" s="4" t="s">
         <v>131</v>
       </c>
       <c r="B115" s="2" t="s">
@@ -6133,8 +6085,8 @@
       </c>
       <c r="C115" s="3"/>
     </row>
-    <row r="116" ht="17.75" spans="1:3">
-      <c r="A116" s="6" t="s">
+    <row r="116" ht="17" spans="1:3">
+      <c r="A116" s="4" t="s">
         <v>131</v>
       </c>
       <c r="B116" s="2" t="s">
@@ -6142,8 +6094,8 @@
       </c>
       <c r="C116" s="3"/>
     </row>
-    <row r="117" ht="17.75" spans="1:3">
-      <c r="A117" s="6" t="s">
+    <row r="117" ht="17" spans="1:3">
+      <c r="A117" s="4" t="s">
         <v>131</v>
       </c>
       <c r="B117" s="2" t="s">
@@ -6151,8 +6103,8 @@
       </c>
       <c r="C117" s="3"/>
     </row>
-    <row r="118" ht="17.75" spans="1:3">
-      <c r="A118" s="6" t="s">
+    <row r="118" ht="17" spans="1:3">
+      <c r="A118" s="4" t="s">
         <v>131</v>
       </c>
       <c r="B118" s="2" t="s">
@@ -6160,8 +6112,8 @@
       </c>
       <c r="C118" s="3"/>
     </row>
-    <row r="119" ht="17.75" spans="1:3">
-      <c r="A119" s="6" t="s">
+    <row r="119" ht="17" spans="1:3">
+      <c r="A119" s="4" t="s">
         <v>131</v>
       </c>
       <c r="B119" s="2" t="s">
@@ -6169,8 +6121,8 @@
       </c>
       <c r="C119" s="3"/>
     </row>
-    <row r="120" ht="17.75" spans="1:3">
-      <c r="A120" s="6" t="s">
+    <row r="120" ht="17" spans="1:3">
+      <c r="A120" s="4" t="s">
         <v>131</v>
       </c>
       <c r="B120" s="2" t="s">
@@ -6178,8 +6130,8 @@
       </c>
       <c r="C120" s="3"/>
     </row>
-    <row r="121" ht="17.75" spans="1:3">
-      <c r="A121" s="6" t="s">
+    <row r="121" ht="17" spans="1:3">
+      <c r="A121" s="4" t="s">
         <v>131</v>
       </c>
       <c r="B121" s="2" t="s">
@@ -6187,8 +6139,8 @@
       </c>
       <c r="C121" s="3"/>
     </row>
-    <row r="122" ht="17.75" spans="1:3">
-      <c r="A122" s="6" t="s">
+    <row r="122" ht="17" spans="1:3">
+      <c r="A122" s="4" t="s">
         <v>131</v>
       </c>
       <c r="B122" s="2" t="s">
@@ -6196,8 +6148,8 @@
       </c>
       <c r="C122" s="3"/>
     </row>
-    <row r="123" ht="17.75" spans="1:3">
-      <c r="A123" s="6" t="s">
+    <row r="123" ht="17" spans="1:3">
+      <c r="A123" s="4" t="s">
         <v>131</v>
       </c>
       <c r="B123" s="2" t="s">
@@ -6205,8 +6157,8 @@
       </c>
       <c r="C123" s="3"/>
     </row>
-    <row r="124" ht="17.75" spans="1:3">
-      <c r="A124" s="6" t="s">
+    <row r="124" ht="17" spans="1:3">
+      <c r="A124" s="4" t="s">
         <v>131</v>
       </c>
       <c r="B124" s="2" t="s">
@@ -6214,8 +6166,8 @@
       </c>
       <c r="C124" s="3"/>
     </row>
-    <row r="125" ht="17.75" spans="1:3">
-      <c r="A125" s="6" t="s">
+    <row r="125" ht="17" spans="1:3">
+      <c r="A125" s="4" t="s">
         <v>131</v>
       </c>
       <c r="B125" s="2" t="s">
@@ -6223,8 +6175,8 @@
       </c>
       <c r="C125" s="3"/>
     </row>
-    <row r="126" ht="17.75" spans="1:3">
-      <c r="A126" s="6" t="s">
+    <row r="126" ht="17" spans="1:3">
+      <c r="A126" s="4" t="s">
         <v>131</v>
       </c>
       <c r="B126" s="2" t="s">
@@ -6232,8 +6184,8 @@
       </c>
       <c r="C126" s="3"/>
     </row>
-    <row r="127" ht="17.75" spans="1:3">
-      <c r="A127" s="6" t="s">
+    <row r="127" ht="17" spans="1:3">
+      <c r="A127" s="4" t="s">
         <v>131</v>
       </c>
       <c r="B127" s="2" t="s">
@@ -6241,8 +6193,8 @@
       </c>
       <c r="C127" s="3"/>
     </row>
-    <row r="128" ht="17.75" spans="1:3">
-      <c r="A128" s="6" t="s">
+    <row r="128" ht="17" spans="1:3">
+      <c r="A128" s="4" t="s">
         <v>131</v>
       </c>
       <c r="B128" s="2" t="s">
@@ -6250,8 +6202,8 @@
       </c>
       <c r="C128" s="3"/>
     </row>
-    <row r="129" ht="17.75" spans="1:3">
-      <c r="A129" s="6" t="s">
+    <row r="129" ht="17" spans="1:3">
+      <c r="A129" s="4" t="s">
         <v>131</v>
       </c>
       <c r="B129" s="2" t="s">
@@ -6259,8 +6211,8 @@
       </c>
       <c r="C129" s="3"/>
     </row>
-    <row r="130" ht="17.75" spans="1:3">
-      <c r="A130" s="6" t="s">
+    <row r="130" ht="17" spans="1:3">
+      <c r="A130" s="4" t="s">
         <v>131</v>
       </c>
       <c r="B130" s="2" t="s">
@@ -6268,8 +6220,8 @@
       </c>
       <c r="C130" s="3"/>
     </row>
-    <row r="131" ht="17.75" spans="1:3">
-      <c r="A131" s="6" t="s">
+    <row r="131" ht="17" spans="1:3">
+      <c r="A131" s="4" t="s">
         <v>131</v>
       </c>
       <c r="B131" s="2" t="s">
@@ -6277,8 +6229,8 @@
       </c>
       <c r="C131" s="3"/>
     </row>
-    <row r="132" ht="17.75" spans="1:3">
-      <c r="A132" s="6" t="s">
+    <row r="132" ht="17" spans="1:3">
+      <c r="A132" s="4" t="s">
         <v>131</v>
       </c>
       <c r="B132" s="2" t="s">
@@ -6286,8 +6238,8 @@
       </c>
       <c r="C132" s="3"/>
     </row>
-    <row r="133" ht="17.75" spans="1:3">
-      <c r="A133" s="6" t="s">
+    <row r="133" ht="17" spans="1:3">
+      <c r="A133" s="4" t="s">
         <v>131</v>
       </c>
       <c r="B133" s="2" t="s">
@@ -6295,8 +6247,8 @@
       </c>
       <c r="C133" s="3"/>
     </row>
-    <row r="134" ht="17.75" spans="1:3">
-      <c r="A134" s="6" t="s">
+    <row r="134" ht="17" spans="1:3">
+      <c r="A134" s="4" t="s">
         <v>131</v>
       </c>
       <c r="B134" s="2" t="s">
@@ -6304,8 +6256,8 @@
       </c>
       <c r="C134" s="3"/>
     </row>
-    <row r="135" ht="17.75" spans="1:3">
-      <c r="A135" s="6" t="s">
+    <row r="135" ht="17" spans="1:3">
+      <c r="A135" s="4" t="s">
         <v>131</v>
       </c>
       <c r="B135" s="2" t="s">
@@ -6313,8 +6265,8 @@
       </c>
       <c r="C135" s="3"/>
     </row>
-    <row r="136" ht="17.75" spans="1:3">
-      <c r="A136" s="6" t="s">
+    <row r="136" ht="17" spans="1:3">
+      <c r="A136" s="4" t="s">
         <v>131</v>
       </c>
       <c r="B136" s="2" t="s">
@@ -6322,8 +6274,8 @@
       </c>
       <c r="C136" s="3"/>
     </row>
-    <row r="137" ht="17.75" spans="1:3">
-      <c r="A137" s="6" t="s">
+    <row r="137" ht="17" spans="1:3">
+      <c r="A137" s="4" t="s">
         <v>131</v>
       </c>
       <c r="B137" s="2" t="s">
@@ -6331,8 +6283,8 @@
       </c>
       <c r="C137" s="3"/>
     </row>
-    <row r="138" ht="17.75" spans="1:3">
-      <c r="A138" s="6" t="s">
+    <row r="138" ht="17" spans="1:3">
+      <c r="A138" s="4" t="s">
         <v>131</v>
       </c>
       <c r="B138" s="2" t="s">
@@ -6340,8 +6292,8 @@
       </c>
       <c r="C138" s="3"/>
     </row>
-    <row r="139" ht="17.75" spans="1:3">
-      <c r="A139" s="6" t="s">
+    <row r="139" ht="17" spans="1:3">
+      <c r="A139" s="4" t="s">
         <v>131</v>
       </c>
       <c r="B139" s="2" t="s">
@@ -6349,8 +6301,8 @@
       </c>
       <c r="C139" s="3"/>
     </row>
-    <row r="140" ht="17.75" spans="1:3">
-      <c r="A140" s="6" t="s">
+    <row r="140" ht="17" spans="1:3">
+      <c r="A140" s="4" t="s">
         <v>131</v>
       </c>
       <c r="B140" s="2" t="s">
@@ -6358,8 +6310,8 @@
       </c>
       <c r="C140" s="3"/>
     </row>
-    <row r="141" ht="17.75" spans="1:3">
-      <c r="A141" s="6" t="s">
+    <row r="141" ht="17" spans="1:3">
+      <c r="A141" s="4" t="s">
         <v>131</v>
       </c>
       <c r="B141" s="2" t="s">
@@ -6367,8 +6319,8 @@
       </c>
       <c r="C141" s="3"/>
     </row>
-    <row r="142" ht="17.75" spans="1:3">
-      <c r="A142" s="6" t="s">
+    <row r="142" ht="17" spans="1:3">
+      <c r="A142" s="4" t="s">
         <v>131</v>
       </c>
       <c r="B142" s="2" t="s">
@@ -6376,8 +6328,8 @@
       </c>
       <c r="C142" s="3"/>
     </row>
-    <row r="143" ht="17.75" spans="1:3">
-      <c r="A143" s="6" t="s">
+    <row r="143" ht="17" spans="1:3">
+      <c r="A143" s="4" t="s">
         <v>131</v>
       </c>
       <c r="B143" s="2" t="s">
@@ -6387,8 +6339,8 @@
         <v>163</v>
       </c>
     </row>
-    <row r="144" ht="17.75" spans="1:3">
-      <c r="A144" s="6" t="s">
+    <row r="144" ht="17" spans="1:3">
+      <c r="A144" s="4" t="s">
         <v>131</v>
       </c>
       <c r="B144" s="2" t="s">
@@ -6396,8 +6348,8 @@
       </c>
       <c r="C144" s="3"/>
     </row>
-    <row r="145" ht="17.75" spans="1:3">
-      <c r="A145" s="6" t="s">
+    <row r="145" ht="17" spans="1:3">
+      <c r="A145" s="4" t="s">
         <v>131</v>
       </c>
       <c r="B145" s="2" t="s">
@@ -6405,8 +6357,8 @@
       </c>
       <c r="C145" s="3"/>
     </row>
-    <row r="146" ht="17.75" spans="1:3">
-      <c r="A146" s="6" t="s">
+    <row r="146" ht="17" spans="1:3">
+      <c r="A146" s="4" t="s">
         <v>131</v>
       </c>
       <c r="B146" s="2" t="s">
@@ -6414,8 +6366,8 @@
       </c>
       <c r="C146" s="3"/>
     </row>
-    <row r="147" ht="17.75" spans="1:3">
-      <c r="A147" s="6" t="s">
+    <row r="147" ht="17" spans="1:3">
+      <c r="A147" s="4" t="s">
         <v>131</v>
       </c>
       <c r="B147" s="2" t="s">
@@ -6425,8 +6377,8 @@
         <v>168</v>
       </c>
     </row>
-    <row r="148" ht="17.75" spans="1:3">
-      <c r="A148" s="6" t="s">
+    <row r="148" ht="17" spans="1:3">
+      <c r="A148" s="4" t="s">
         <v>131</v>
       </c>
       <c r="B148" s="2" t="s">
@@ -6434,7 +6386,7 @@
       </c>
       <c r="C148" s="3"/>
     </row>
-    <row r="149" ht="17.75" spans="1:3">
+    <row r="149" ht="17" spans="1:3">
       <c r="A149" s="4" t="s">
         <v>131</v>
       </c>
@@ -6452,7 +6404,7 @@
       </c>
       <c r="C150" s="3"/>
     </row>
-    <row r="151" ht="17.75" spans="1:3">
+    <row r="151" ht="17" spans="1:3">
       <c r="A151" s="4" t="s">
         <v>171</v>
       </c>
@@ -6461,7 +6413,7 @@
       </c>
       <c r="C151" s="3"/>
     </row>
-    <row r="152" ht="17.75" spans="1:3">
+    <row r="152" ht="17" spans="1:3">
       <c r="A152" s="4" t="s">
         <v>171</v>
       </c>
@@ -6470,7 +6422,7 @@
       </c>
       <c r="C152" s="3"/>
     </row>
-    <row r="153" ht="17.75" spans="1:3">
+    <row r="153" ht="17" spans="1:3">
       <c r="A153" s="4" t="s">
         <v>171</v>
       </c>
@@ -6481,7 +6433,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="154" ht="17.75" spans="1:3">
+    <row r="154" ht="17" spans="1:3">
       <c r="A154" s="4" t="s">
         <v>171</v>
       </c>
@@ -6490,7 +6442,7 @@
       </c>
       <c r="C154" s="3"/>
     </row>
-    <row r="155" ht="17.75" spans="1:3">
+    <row r="155" ht="17" spans="1:3">
       <c r="A155" s="4" t="s">
         <v>171</v>
       </c>
@@ -6499,25 +6451,14 @@
       </c>
       <c r="C155" s="3"/>
     </row>
-    <row r="156" ht="17.75" spans="1:3">
+    <row r="156" ht="17" spans="1:3">
       <c r="A156" s="4" t="s">
         <v>171</v>
       </c>
       <c r="B156" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="C156" s="8"/>
-    </row>
-    <row r="158" spans="1:3">
-      <c r="A158">
-        <v>12344</v>
-      </c>
-      <c r="B158" t="s">
-        <v>179</v>
-      </c>
-      <c r="C158" t="s">
-        <v>180</v>
-      </c>
+      <c r="C156" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
自动更新数据 - 2025-04-28 20:53:21
</commit_message>
<xml_diff>
--- a/data/raw/水晶.xlsx
+++ b/data/raw/水晶.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="180">
   <si>
     <t>名称</t>
   </si>
@@ -249,6 +249,83 @@
     <t>独山玉</t>
   </si>
   <si>
+    <r>
+      <t>翡翠</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ 明朝"/>
+        <charset val="134"/>
+      </rPr>
+      <t>和田玉</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ 明朝"/>
+        <charset val="134"/>
+      </rPr>
+      <t>其他玉石</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>----</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ 明朝"/>
+        <charset val="134"/>
+      </rPr>
+      <t>其他天然玉石</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>---</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ 明朝"/>
+        <charset val="134"/>
+      </rPr>
+      <t>多宝玉石</t>
+    </r>
+  </si>
+  <si>
     <t>石英质玉</t>
   </si>
   <si>
@@ -3813,7 +3890,7 @@
     <t>发晶</t>
   </si>
   <si>
-    <t>紫水晶，兔毛，粉水晶，黄水晶，彩发晶</t>
+    <t>紫水晶，兔毛，粉水晶，黄水晶，彩发晶，白幽灵</t>
   </si>
   <si>
     <t>紫晶</t>
@@ -5015,8 +5092,8 @@
   <sheetPr/>
   <dimension ref="A1:C156"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="119" workbookViewId="0">
-      <selection activeCell="A159" sqref="$A1:$XFD1048576"/>
+    <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="119" topLeftCell="A141" workbookViewId="0">
+      <selection activeCell="D155" sqref="D155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelCol="2"/>
@@ -5147,13 +5224,13 @@
     </row>
     <row r="14" ht="17" spans="1:3">
       <c r="A14" s="4" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" ht="17" spans="1:3">
@@ -5161,7 +5238,7 @@
         <v>5</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C15" s="3"/>
     </row>
@@ -5170,7 +5247,7 @@
         <v>5</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C16" s="3"/>
     </row>
@@ -5179,7 +5256,7 @@
         <v>5</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C17" s="3"/>
     </row>
@@ -5188,7 +5265,7 @@
         <v>5</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C18" s="3"/>
     </row>
@@ -5197,7 +5274,7 @@
         <v>5</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C19" s="3"/>
     </row>
@@ -5206,10 +5283,10 @@
         <v>5</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" ht="17" spans="1:3">
@@ -5217,7 +5294,7 @@
         <v>5</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C21" s="3"/>
     </row>
@@ -5226,7 +5303,7 @@
         <v>5</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C22" s="3"/>
     </row>
@@ -5235,7 +5312,7 @@
         <v>5</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C23" s="3"/>
     </row>
@@ -5244,10 +5321,10 @@
         <v>5</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" ht="17" spans="1:3">
@@ -5255,7 +5332,7 @@
         <v>5</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C25" s="3"/>
     </row>
@@ -5264,7 +5341,7 @@
         <v>5</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C26" s="3"/>
     </row>
@@ -5273,7 +5350,7 @@
         <v>5</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C27" s="3"/>
     </row>
@@ -5282,13 +5359,13 @@
         <v>5</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C28" s="3"/>
     </row>
     <row r="29" ht="17" spans="1:3">
       <c r="A29" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>16</v>
@@ -5297,18 +5374,18 @@
     </row>
     <row r="30" ht="84" customHeight="1" spans="1:3">
       <c r="A30" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" ht="17" spans="1:3">
       <c r="A31" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>14</v>
@@ -5317,27 +5394,27 @@
     </row>
     <row r="32" ht="17" spans="1:3">
       <c r="A32" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" ht="17" spans="1:3">
       <c r="A33" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C33" s="3"/>
     </row>
     <row r="34" ht="17" spans="1:3">
       <c r="A34" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>10</v>
@@ -5346,7 +5423,7 @@
     </row>
     <row r="35" ht="17" spans="1:3">
       <c r="A35" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>11</v>
@@ -5355,72 +5432,72 @@
     </row>
     <row r="36" ht="17" spans="1:3">
       <c r="A36" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37" ht="18.5" customHeight="1" spans="1:3">
       <c r="A37" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C37" s="3"/>
     </row>
     <row r="38" ht="17" spans="1:3">
       <c r="A38" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C38" s="3"/>
     </row>
     <row r="39" ht="17" spans="1:3">
       <c r="A39" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C39" s="3"/>
     </row>
     <row r="40" ht="17" spans="1:3">
       <c r="A40" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C40" s="3"/>
     </row>
     <row r="41" ht="17" spans="1:3">
       <c r="A41" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C41" s="3"/>
     </row>
     <row r="42" ht="17" spans="1:3">
       <c r="A42" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C42" s="3"/>
     </row>
     <row r="43" ht="17" spans="1:3">
       <c r="A43" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>12</v>
@@ -5429,180 +5506,180 @@
     </row>
     <row r="44" ht="52.5" customHeight="1" spans="1:3">
       <c r="A44" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C44" s="3"/>
     </row>
     <row r="45" ht="17" spans="1:3">
       <c r="A45" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C45" s="3"/>
     </row>
     <row r="46" ht="17" spans="1:3">
       <c r="A46" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C46" s="3"/>
     </row>
     <row r="47" ht="17" spans="1:3">
       <c r="A47" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C47" s="3"/>
     </row>
     <row r="48" ht="17" spans="1:3">
       <c r="A48" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C48" s="3"/>
     </row>
     <row r="49" ht="17" spans="1:3">
       <c r="A49" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C49" s="3"/>
     </row>
     <row r="50" ht="17" spans="1:3">
       <c r="A50" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C50" s="3"/>
     </row>
     <row r="51" ht="17" spans="1:3">
       <c r="A51" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C51" s="3"/>
     </row>
     <row r="52" ht="17" spans="1:3">
       <c r="A52" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C52" s="3"/>
     </row>
     <row r="53" ht="17" spans="1:3">
       <c r="A53" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C53" s="3"/>
     </row>
     <row r="54" ht="17" spans="1:3">
       <c r="A54" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="55" ht="17" spans="1:3">
       <c r="A55" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C55" s="3"/>
     </row>
     <row r="56" ht="17" spans="1:3">
       <c r="A56" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C56" s="3"/>
     </row>
     <row r="57" ht="17" spans="1:3">
       <c r="A57" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C57" s="3"/>
     </row>
     <row r="58" ht="17" spans="1:3">
       <c r="A58" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C58" s="3"/>
     </row>
     <row r="59" ht="17" spans="1:3">
       <c r="A59" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C59" s="3"/>
     </row>
     <row r="60" ht="17" spans="1:3">
       <c r="A60" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C60" s="3"/>
     </row>
     <row r="61" ht="17" spans="1:3">
       <c r="A61" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C61" s="3"/>
     </row>
     <row r="62" ht="17" spans="1:3">
       <c r="A62" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C62" s="3"/>
     </row>
     <row r="63" ht="35.5" customHeight="1" spans="1:3">
       <c r="A63" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>8</v>
@@ -5611,7 +5688,7 @@
     </row>
     <row r="64" ht="17" spans="1:3">
       <c r="A64" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>13</v>
@@ -5620,843 +5697,843 @@
     </row>
     <row r="65" ht="17" spans="1:3">
       <c r="A65" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C65" s="3"/>
     </row>
     <row r="66" ht="17" spans="1:3">
       <c r="A66" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C66" s="3"/>
     </row>
     <row r="67" ht="18.5" customHeight="1" spans="1:3">
       <c r="A67" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C67" s="3"/>
     </row>
     <row r="68" ht="17" spans="1:3">
       <c r="A68" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C68" s="3"/>
     </row>
     <row r="69" ht="17" spans="1:3">
       <c r="A69" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C69" s="3"/>
     </row>
     <row r="70" ht="17" spans="1:3">
       <c r="A70" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="71" ht="17" spans="1:3">
       <c r="A71" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C71" s="3"/>
     </row>
     <row r="72" ht="17" spans="1:3">
       <c r="A72" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C72" s="3"/>
     </row>
     <row r="73" ht="17" spans="1:3">
       <c r="A73" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C73" s="3"/>
     </row>
     <row r="74" ht="17" spans="1:3">
       <c r="A74" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C74" s="3"/>
     </row>
     <row r="75" ht="56" customHeight="1" spans="1:3">
       <c r="A75" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="76" ht="17" spans="1:3">
       <c r="A76" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C76" s="3"/>
     </row>
     <row r="77" ht="17" spans="1:3">
       <c r="A77" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C77" s="3"/>
     </row>
     <row r="78" ht="17" spans="1:3">
       <c r="A78" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C78" s="3"/>
     </row>
     <row r="79" ht="17" spans="1:3">
       <c r="A79" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C79" s="3"/>
     </row>
     <row r="80" ht="17" spans="1:3">
       <c r="A80" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C80" s="3"/>
     </row>
     <row r="81" ht="17" spans="1:3">
       <c r="A81" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C81" s="3"/>
     </row>
     <row r="82" ht="17" spans="1:3">
       <c r="A82" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C82" s="3"/>
     </row>
     <row r="83" ht="17" spans="1:3">
       <c r="A83" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C83" s="3"/>
     </row>
     <row r="84" ht="17" spans="1:3">
       <c r="A84" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C84" s="3"/>
     </row>
     <row r="85" ht="17" spans="1:3">
       <c r="A85" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C85" s="3"/>
     </row>
     <row r="86" ht="17" spans="1:3">
       <c r="A86" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C86" s="3"/>
     </row>
     <row r="87" ht="17" spans="1:3">
       <c r="A87" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C87" s="3"/>
     </row>
     <row r="88" ht="17" spans="1:3">
       <c r="A88" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C88" s="3"/>
     </row>
     <row r="89" ht="17" spans="1:3">
       <c r="A89" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C89" s="3"/>
     </row>
     <row r="90" ht="81.5" customHeight="1" spans="1:3">
       <c r="A90" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C90" s="3"/>
     </row>
     <row r="91" ht="34" spans="1:3">
       <c r="A91" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C91" s="3"/>
     </row>
     <row r="92" ht="34" spans="1:3">
       <c r="A92" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C92" s="3"/>
     </row>
     <row r="93" ht="34" spans="1:3">
       <c r="A93" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C93" s="3"/>
     </row>
     <row r="94" ht="67" customHeight="1" spans="1:3">
       <c r="A94" s="4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C94" s="3"/>
     </row>
     <row r="95" ht="17" spans="1:3">
       <c r="A95" s="4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C95" s="3"/>
     </row>
     <row r="96" ht="101" customHeight="1" spans="1:3">
       <c r="A96" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C96" s="3"/>
     </row>
     <row r="97" ht="17" spans="1:3">
       <c r="A97" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C97" s="3"/>
     </row>
     <row r="98" ht="17" spans="1:3">
       <c r="A98" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C98" s="3"/>
     </row>
     <row r="99" ht="17" spans="1:3">
       <c r="A99" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="100" ht="160.5" customHeight="1" spans="1:3">
       <c r="A100" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="101" ht="34" spans="1:3">
       <c r="A101" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C101" s="3"/>
     </row>
     <row r="102" ht="34" spans="1:3">
       <c r="A102" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C102" s="3"/>
     </row>
     <row r="103" ht="34" spans="1:3">
       <c r="A103" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C103" s="3"/>
     </row>
     <row r="104" ht="34" spans="1:3">
       <c r="A104" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C104" s="3"/>
     </row>
     <row r="105" ht="18.5" customHeight="1" spans="1:3">
       <c r="A105" s="4" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C105" s="3"/>
     </row>
     <row r="106" ht="17" spans="1:3">
       <c r="A106" s="4" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C106" s="3"/>
     </row>
     <row r="107" ht="17" spans="1:3">
       <c r="A107" s="4" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C107" s="3"/>
     </row>
     <row r="108" ht="17" spans="1:3">
       <c r="A108" s="4" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C108" s="3"/>
     </row>
     <row r="109" ht="17" spans="1:3">
       <c r="A109" s="4" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C109" s="3"/>
     </row>
     <row r="110" ht="17" spans="1:3">
       <c r="A110" s="4" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C110" s="3"/>
     </row>
     <row r="111" ht="84" customHeight="1" spans="1:3">
       <c r="A111" s="4" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C111" s="3"/>
     </row>
     <row r="112" ht="17" spans="1:3">
       <c r="A112" s="4" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C112" s="3"/>
     </row>
     <row r="113" ht="69.5" customHeight="1" spans="1:3">
       <c r="A113" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C113" s="3"/>
     </row>
     <row r="114" ht="17" spans="1:3">
       <c r="A114" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C114" s="3"/>
     </row>
     <row r="115" ht="17" spans="1:3">
       <c r="A115" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C115" s="3"/>
     </row>
     <row r="116" ht="17" spans="1:3">
       <c r="A116" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C116" s="3"/>
     </row>
     <row r="117" ht="17" spans="1:3">
       <c r="A117" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C117" s="3"/>
     </row>
     <row r="118" ht="17" spans="1:3">
       <c r="A118" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C118" s="3"/>
     </row>
     <row r="119" ht="17" spans="1:3">
       <c r="A119" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C119" s="3"/>
     </row>
     <row r="120" ht="17" spans="1:3">
       <c r="A120" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C120" s="3"/>
     </row>
     <row r="121" ht="17" spans="1:3">
       <c r="A121" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C121" s="3"/>
     </row>
     <row r="122" ht="17" spans="1:3">
       <c r="A122" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C122" s="3"/>
     </row>
     <row r="123" ht="17" spans="1:3">
       <c r="A123" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C123" s="3"/>
     </row>
     <row r="124" ht="17" spans="1:3">
       <c r="A124" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C124" s="3"/>
     </row>
     <row r="125" ht="17" spans="1:3">
       <c r="A125" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C125" s="3"/>
     </row>
     <row r="126" ht="17" spans="1:3">
       <c r="A126" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C126" s="3"/>
     </row>
     <row r="127" ht="17" spans="1:3">
       <c r="A127" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C127" s="3"/>
     </row>
     <row r="128" ht="17" spans="1:3">
       <c r="A128" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C128" s="3"/>
     </row>
     <row r="129" ht="17" spans="1:3">
       <c r="A129" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C129" s="3"/>
     </row>
     <row r="130" ht="17" spans="1:3">
       <c r="A130" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C130" s="3"/>
     </row>
     <row r="131" ht="17" spans="1:3">
       <c r="A131" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C131" s="3"/>
     </row>
     <row r="132" ht="17" spans="1:3">
       <c r="A132" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C132" s="3"/>
     </row>
     <row r="133" ht="17" spans="1:3">
       <c r="A133" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C133" s="3"/>
     </row>
     <row r="134" ht="17" spans="1:3">
       <c r="A134" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C134" s="3"/>
     </row>
     <row r="135" ht="17" spans="1:3">
       <c r="A135" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C135" s="3"/>
     </row>
     <row r="136" ht="17" spans="1:3">
       <c r="A136" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C136" s="3"/>
     </row>
     <row r="137" ht="17" spans="1:3">
       <c r="A137" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C137" s="3"/>
     </row>
     <row r="138" ht="17" spans="1:3">
       <c r="A138" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C138" s="3"/>
     </row>
     <row r="139" ht="17" spans="1:3">
       <c r="A139" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C139" s="3"/>
     </row>
     <row r="140" ht="17" spans="1:3">
       <c r="A140" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C140" s="3"/>
     </row>
     <row r="141" ht="17" spans="1:3">
       <c r="A141" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C141" s="3"/>
     </row>
     <row r="142" ht="17" spans="1:3">
       <c r="A142" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C142" s="3"/>
     </row>
     <row r="143" ht="17" spans="1:3">
       <c r="A143" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C143" s="5" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="144" ht="17" spans="1:3">
       <c r="A144" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C144" s="3"/>
     </row>
     <row r="145" ht="17" spans="1:3">
       <c r="A145" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C145" s="3"/>
     </row>
     <row r="146" ht="17" spans="1:3">
       <c r="A146" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C146" s="3"/>
     </row>
     <row r="147" ht="17" spans="1:3">
       <c r="A147" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C147" s="5" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="148" ht="17" spans="1:3">
       <c r="A148" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C148" s="3"/>
     </row>
     <row r="149" ht="17" spans="1:3">
       <c r="A149" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C149" s="3"/>
     </row>
     <row r="150" ht="18.5" customHeight="1" spans="1:3">
       <c r="A150" s="4" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C150" s="3"/>
     </row>
     <row r="151" ht="17" spans="1:3">
       <c r="A151" s="4" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C151" s="3"/>
     </row>
     <row r="152" ht="17" spans="1:3">
       <c r="A152" s="4" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C152" s="3"/>
     </row>
-    <row r="153" ht="17" spans="1:3">
+    <row r="153" ht="34" spans="1:3">
       <c r="A153" s="4" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B153" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C153" s="5" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="154" ht="17" spans="1:3">
       <c r="A154" s="4" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C154" s="3"/>
     </row>
     <row r="155" ht="17" spans="1:3">
       <c r="A155" s="4" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C155" s="3"/>
     </row>
     <row r="156" ht="17" spans="1:3">
       <c r="A156" s="4" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C156" s="7"/>
     </row>

</xml_diff>

<commit_message>
自动更新数据 - 2025-04-30 23:10:00
</commit_message>
<xml_diff>
--- a/data/raw/水晶.xlsx
+++ b/data/raw/水晶.xlsx
@@ -3813,7 +3813,7 @@
     <t>发晶</t>
   </si>
   <si>
-    <t>紫水晶，兔毛，粉水晶，黄水晶，彩发晶，白幽灵，白水晶，金发晶，马粉，四季幽灵，石榴石，红幽灵</t>
+    <t>紫水晶，兔毛，粉水晶，黄水晶，彩发晶，白幽灵，白水晶，金发晶，马粉，四季幽灵，石榴石，红幽灵，粉晶，</t>
   </si>
   <si>
     <t>紫晶</t>
@@ -5016,7 +5016,7 @@
   <dimension ref="A1:C156"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="119" topLeftCell="A146" workbookViewId="0">
-      <selection activeCell="C156" sqref="D156 C156"/>
+      <selection activeCell="D153" sqref="D153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelCol="2"/>

</xml_diff>

<commit_message>
自动更新数据 - 2025-04-30 23:45:39
</commit_message>
<xml_diff>
--- a/data/raw/水晶.xlsx
+++ b/data/raw/水晶.xlsx
@@ -3813,7 +3813,7 @@
     <t>发晶</t>
   </si>
   <si>
-    <t>紫水晶，兔毛，粉水晶，黄水晶，彩发晶，白幽灵，白水晶，金发晶，马粉，四季幽灵，石榴石，红幽灵，粉晶，</t>
+    <t>紫水晶，兔毛，粉水晶，黄水晶，彩发晶，白幽灵，白水晶，金发晶，马粉，四季幽灵，石榴石，红幽灵，粉晶，毒液，超七，绿月光，蓝针</t>
   </si>
   <si>
     <t>紫晶</t>
@@ -5015,8 +5015,8 @@
   <sheetPr/>
   <dimension ref="A1:C156"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="119" topLeftCell="A146" workbookViewId="0">
-      <selection activeCell="D153" sqref="D153"/>
+    <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="119" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="F156" sqref="F156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelCol="2"/>
@@ -6422,7 +6422,7 @@
       </c>
       <c r="C152" s="3"/>
     </row>
-    <row r="153" ht="51" spans="1:3">
+    <row r="153" ht="68" spans="1:3">
       <c r="A153" s="4" t="s">
         <v>171</v>
       </c>

</xml_diff>

<commit_message>
自动更新数据 - 2025-04-30 23:58:20
</commit_message>
<xml_diff>
--- a/data/raw/水晶.xlsx
+++ b/data/raw/水晶.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="180">
   <si>
     <t>名称</t>
   </si>
@@ -3823,6 +3823,9 @@
   </si>
   <si>
     <t>芙蓉石</t>
+  </si>
+  <si>
+    <t>卫金权</t>
   </si>
 </sst>
 </file>
@@ -5016,7 +5019,7 @@
   <dimension ref="A1:C156"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="119" topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="F156" sqref="F156"/>
+      <selection activeCell="C157" sqref="C157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelCol="2"/>
@@ -6458,7 +6461,9 @@
       <c r="B156" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="C156" s="7"/>
+      <c r="C156" s="7" t="s">
+        <v>179</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
自动更新数据 - 2025-05-01 00:03:14
</commit_message>
<xml_diff>
--- a/data/raw/水晶.xlsx
+++ b/data/raw/水晶.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="179">
   <si>
     <t>名称</t>
   </si>
@@ -3823,9 +3823,6 @@
   </si>
   <si>
     <t>芙蓉石</t>
-  </si>
-  <si>
-    <t>卫金权</t>
   </si>
 </sst>
 </file>
@@ -5018,8 +5015,8 @@
   <sheetPr/>
   <dimension ref="A1:C156"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="119" topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="C157" sqref="C157"/>
+    <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="119" topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="C159" sqref="C159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelCol="2"/>
@@ -6461,9 +6458,7 @@
       <c r="B156" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="C156" s="7" t="s">
-        <v>179</v>
-      </c>
+      <c r="C156" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
自动更新数据 - 2025-05-02 21:39:18
</commit_message>
<xml_diff>
--- a/data/raw/水晶.xlsx
+++ b/data/raw/水晶.xlsx
@@ -3686,12 +3686,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="ＭＳ 明朝"/>
-        <charset val="134"/>
-      </rPr>
       <t>黄金</t>
     </r>
     <r>
@@ -3725,10 +3719,19 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ 明朝"/>
-        <charset val="134"/>
-      </rPr>
-      <t>钻石</t>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>钻</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ 明朝"/>
+        <charset val="134"/>
+      </rPr>
+      <t>石</t>
     </r>
     <r>
       <rPr>
@@ -3747,42 +3750,6 @@
         <charset val="134"/>
       </rPr>
       <t>珍珠</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Cambria"/>
-        <charset val="134"/>
-      </rPr>
-      <t>--</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="ＭＳ 明朝"/>
-        <charset val="134"/>
-      </rPr>
-      <t>彩色宝石</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Cambria"/>
-        <charset val="134"/>
-      </rPr>
-      <t>/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="ＭＳ 明朝"/>
-        <charset val="134"/>
-      </rPr>
-      <t>贵重宝石</t>
     </r>
     <r>
       <rPr>
@@ -5015,8 +4982,8 @@
   <sheetPr/>
   <dimension ref="A1:C156"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="119" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="C159" sqref="C159"/>
+    <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="119" topLeftCell="A141" workbookViewId="0">
+      <selection activeCell="C157" sqref="C157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelCol="2"/>

</xml_diff>